<commit_message>
chat with your tickets
</commit_message>
<xml_diff>
--- a/backend/data/Liite 3 Datahub Muutostoiveet 20240816.xlsx
+++ b/backend/data/Liite 3 Datahub Muutostoiveet 20240816.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Fingrid\Kehitystyöryhmän toiminta\Kokoukset\20240903\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sagar/Desktop/Junction/FinGrid/backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D755029-F44A-4D58-A3CB-501DE3584552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959057C2-B3AD-1D43-B9C7-3AF7244DF608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kehitysehdotukset" sheetId="1" r:id="rId1"/>
@@ -12712,13 +12712,6 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:W425" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
-  <autoFilter ref="A1:W425" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Kehitysehdotus, tapaaminen 15"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <tableColumns count="23">
     <tableColumn id="17" xr3:uid="{AA7DA508-3563-4FB4-8922-88C62AE6CBFC}" name="ID" dataDxfId="22"/>
     <tableColumn id="18" xr3:uid="{4D97A41E-9DDB-4208-9A45-78A6AFEAC63E}" name="Suunniteltu toteutus-versio_x000a_Planned release version" dataDxfId="21"/>
@@ -13031,38 +13024,38 @@
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A117" sqref="A117"/>
-      <selection pane="topRight" activeCell="M205" sqref="M205"/>
+      <selection pane="topRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="4" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="48.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28.75" style="1" customWidth="1"/>
-    <col min="6" max="6" width="69.75" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.25" style="1" customWidth="1"/>
-    <col min="8" max="8" width="50.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="48.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="69.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="50.1640625" style="1" customWidth="1"/>
     <col min="9" max="9" width="17" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="21.125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="21.1640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="17.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13.625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.6640625" style="1" customWidth="1"/>
     <col min="15" max="15" width="13" style="1" customWidth="1"/>
-    <col min="16" max="16" width="25.125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="25.1640625" style="1" customWidth="1"/>
     <col min="17" max="17" width="21.5" style="1" customWidth="1"/>
-    <col min="18" max="18" width="103.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="103.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="40.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="33.625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="40.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.1640625" style="1" customWidth="1"/>
+    <col min="22" max="22" width="33.6640625" style="1" customWidth="1"/>
     <col min="23" max="23" width="63.5" style="1" customWidth="1"/>
-    <col min="26" max="16384" width="8.625" style="2"/>
+    <col min="26" max="16384" width="8.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="74.849999999999994" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" ht="74.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="17" t="s">
         <v>68</v>
       </c>
@@ -13135,7 +13128,7 @@
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
     </row>
-    <row r="2" spans="1:25" ht="85.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" ht="90" x14ac:dyDescent="0.15">
       <c r="A2" s="33" t="s">
         <v>90</v>
       </c>
@@ -13188,7 +13181,7 @@
       <c r="X2" s="2"/>
       <c r="Y2" s="2"/>
     </row>
-    <row r="3" spans="1:25" ht="285" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" ht="300" x14ac:dyDescent="0.15">
       <c r="A3" s="4">
         <v>3</v>
       </c>
@@ -13245,7 +13238,7 @@
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
     </row>
-    <row r="4" spans="1:25" ht="370.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" ht="384" x14ac:dyDescent="0.15">
       <c r="A4" s="4">
         <v>4</v>
       </c>
@@ -13304,7 +13297,7 @@
       <c r="X4" s="2"/>
       <c r="Y4" s="2"/>
     </row>
-    <row r="5" spans="1:25" ht="162" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" ht="162" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4">
         <v>5</v>
       </c>
@@ -13369,7 +13362,7 @@
       <c r="X5" s="2"/>
       <c r="Y5" s="2"/>
     </row>
-    <row r="6" spans="1:25" ht="163.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" ht="163.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4">
         <v>6</v>
       </c>
@@ -13428,7 +13421,7 @@
       <c r="X6" s="2"/>
       <c r="Y6" s="2"/>
     </row>
-    <row r="7" spans="1:25" ht="96" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" ht="96" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4">
         <v>7</v>
       </c>
@@ -13487,7 +13480,7 @@
       <c r="X7" s="2"/>
       <c r="Y7" s="2"/>
     </row>
-    <row r="8" spans="1:25" ht="213.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" ht="225" x14ac:dyDescent="0.15">
       <c r="A8" s="4">
         <v>8</v>
       </c>
@@ -13544,7 +13537,7 @@
       <c r="X8" s="2"/>
       <c r="Y8" s="2"/>
     </row>
-    <row r="9" spans="1:25" s="3" customFormat="1" ht="147.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" s="3" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="32">
         <v>9</v>
       </c>
@@ -13609,7 +13602,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="215.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" ht="215.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4">
         <v>10</v>
       </c>
@@ -13660,7 +13653,7 @@
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
     </row>
-    <row r="11" spans="1:25" ht="299.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" ht="314" x14ac:dyDescent="0.15">
       <c r="A11" s="4">
         <v>11</v>
       </c>
@@ -13729,7 +13722,7 @@
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
     </row>
-    <row r="12" spans="1:25" ht="137.85" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" ht="137.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4">
         <v>12</v>
       </c>
@@ -13790,7 +13783,7 @@
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
     </row>
-    <row r="13" spans="1:25" ht="185.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" ht="195" x14ac:dyDescent="0.15">
       <c r="A13" s="4">
         <v>13</v>
       </c>
@@ -13841,7 +13834,7 @@
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
     </row>
-    <row r="14" spans="1:25" ht="178.35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" ht="178.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4">
         <v>14</v>
       </c>
@@ -13892,7 +13885,7 @@
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
     </row>
-    <row r="15" spans="1:25" ht="85.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" ht="90" x14ac:dyDescent="0.15">
       <c r="A15" s="4">
         <v>15</v>
       </c>
@@ -13945,7 +13938,7 @@
       <c r="X15" s="2"/>
       <c r="Y15" s="2"/>
     </row>
-    <row r="16" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A16" s="4">
         <v>16</v>
       </c>
@@ -14012,7 +14005,7 @@
       <c r="X16" s="2"/>
       <c r="Y16" s="2"/>
     </row>
-    <row r="17" spans="1:25" ht="156.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" ht="165" x14ac:dyDescent="0.15">
       <c r="A17" s="4">
         <v>17</v>
       </c>
@@ -14075,7 +14068,7 @@
       <c r="X17" s="2"/>
       <c r="Y17" s="2"/>
     </row>
-    <row r="18" spans="1:25" ht="71.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" ht="90" x14ac:dyDescent="0.15">
       <c r="A18" s="4">
         <v>18</v>
       </c>
@@ -14136,7 +14129,7 @@
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
     </row>
-    <row r="19" spans="1:25" ht="187.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" ht="187.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4">
         <v>19</v>
       </c>
@@ -14197,7 +14190,7 @@
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
     </row>
-    <row r="20" spans="1:25" ht="236.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" ht="236.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4">
         <v>20</v>
       </c>
@@ -14252,7 +14245,7 @@
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
     </row>
-    <row r="21" spans="1:25" ht="185.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" ht="195" x14ac:dyDescent="0.15">
       <c r="A21" s="4">
         <v>21</v>
       </c>
@@ -14311,7 +14304,7 @@
       <c r="X21" s="2"/>
       <c r="Y21" s="2"/>
     </row>
-    <row r="22" spans="1:25" ht="133.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" ht="133.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4">
         <v>22</v>
       </c>
@@ -14374,7 +14367,7 @@
       <c r="X22" s="2"/>
       <c r="Y22" s="2"/>
     </row>
-    <row r="23" spans="1:25" ht="156.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" ht="165" x14ac:dyDescent="0.15">
       <c r="A23" s="4">
         <v>23</v>
       </c>
@@ -14429,7 +14422,7 @@
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
     </row>
-    <row r="24" spans="1:25" ht="99.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" ht="105" x14ac:dyDescent="0.15">
       <c r="A24" s="4">
         <v>24</v>
       </c>
@@ -14486,7 +14479,7 @@
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
     </row>
-    <row r="25" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A25" s="4">
         <v>25</v>
       </c>
@@ -14545,7 +14538,7 @@
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
     </row>
-    <row r="26" spans="1:25" ht="180" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" ht="180" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4">
         <v>26</v>
       </c>
@@ -14608,7 +14601,7 @@
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
     </row>
-    <row r="27" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A27" s="4">
         <v>27</v>
       </c>
@@ -14669,7 +14662,7 @@
       <c r="X27" s="2"/>
       <c r="Y27" s="2"/>
     </row>
-    <row r="28" spans="1:25" ht="42.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" ht="45" x14ac:dyDescent="0.15">
       <c r="A28" s="4">
         <v>28</v>
       </c>
@@ -14716,7 +14709,7 @@
       <c r="X28" s="2"/>
       <c r="Y28" s="2"/>
     </row>
-    <row r="29" spans="1:25" ht="28.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" ht="45" x14ac:dyDescent="0.15">
       <c r="A29" s="4">
         <v>29</v>
       </c>
@@ -14761,7 +14754,7 @@
       <c r="X29" s="2"/>
       <c r="Y29" s="2"/>
     </row>
-    <row r="30" spans="1:25" ht="147" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" ht="147" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="4">
         <v>30</v>
       </c>
@@ -14824,7 +14817,7 @@
       <c r="X30" s="2"/>
       <c r="Y30" s="2"/>
     </row>
-    <row r="31" spans="1:25" ht="90" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" ht="90" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="4">
         <v>31</v>
       </c>
@@ -14891,7 +14884,7 @@
       <c r="X31" s="2"/>
       <c r="Y31" s="2"/>
     </row>
-    <row r="32" spans="1:25" ht="251.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" ht="251" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="4">
         <v>32</v>
       </c>
@@ -14948,7 +14941,7 @@
       <c r="X32" s="2"/>
       <c r="Y32" s="2"/>
     </row>
-    <row r="33" spans="1:25" ht="327.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:25" ht="342" x14ac:dyDescent="0.15">
       <c r="A33" s="4">
         <v>33</v>
       </c>
@@ -15015,7 +15008,7 @@
       <c r="X33" s="2"/>
       <c r="Y33" s="2"/>
     </row>
-    <row r="34" spans="1:25" ht="142.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:25" ht="150" x14ac:dyDescent="0.15">
       <c r="A34" s="4">
         <v>34</v>
       </c>
@@ -15074,7 +15067,7 @@
       <c r="X34" s="2"/>
       <c r="Y34" s="2"/>
     </row>
-    <row r="35" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A35" s="4">
         <v>35</v>
       </c>
@@ -15141,7 +15134,7 @@
       <c r="X35" s="2"/>
       <c r="Y35" s="2"/>
     </row>
-    <row r="36" spans="1:25" ht="99.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:25" ht="105" x14ac:dyDescent="0.15">
       <c r="A36" s="4">
         <v>36</v>
       </c>
@@ -15196,7 +15189,7 @@
       <c r="X36" s="2"/>
       <c r="Y36" s="2"/>
     </row>
-    <row r="37" spans="1:25" ht="276.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:25" ht="277" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="4">
         <v>37</v>
       </c>
@@ -15261,7 +15254,7 @@
       <c r="X37" s="2"/>
       <c r="Y37" s="2"/>
     </row>
-    <row r="38" spans="1:25" ht="232.35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:25" ht="232.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="4">
         <v>38</v>
       </c>
@@ -15320,7 +15313,7 @@
       <c r="X38" s="2"/>
       <c r="Y38" s="2"/>
     </row>
-    <row r="39" spans="1:25" ht="166.35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:25" ht="166.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="4">
         <v>39</v>
       </c>
@@ -15383,7 +15376,7 @@
       <c r="X39" s="2"/>
       <c r="Y39" s="2"/>
     </row>
-    <row r="40" spans="1:25" ht="42.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:25" ht="45" x14ac:dyDescent="0.15">
       <c r="A40" s="4">
         <v>40</v>
       </c>
@@ -15442,7 +15435,7 @@
       <c r="X40" s="2"/>
       <c r="Y40" s="2"/>
     </row>
-    <row r="41" spans="1:25" ht="132.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:25" ht="132.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="4">
         <v>41</v>
       </c>
@@ -15509,7 +15502,7 @@
       <c r="X41" s="2"/>
       <c r="Y41" s="2"/>
     </row>
-    <row r="42" spans="1:25" ht="176.85" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:25" ht="176.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="4">
         <v>42</v>
       </c>
@@ -15574,7 +15567,7 @@
       <c r="X42" s="2"/>
       <c r="Y42" s="2"/>
     </row>
-    <row r="43" spans="1:25" ht="113.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:25" ht="113.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="4">
         <v>43</v>
       </c>
@@ -15633,7 +15626,7 @@
       <c r="X43" s="2"/>
       <c r="Y43" s="2"/>
     </row>
-    <row r="44" spans="1:25" ht="185.85" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:25" ht="185.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="4">
         <v>44</v>
       </c>
@@ -15692,7 +15685,7 @@
       <c r="X44" s="2"/>
       <c r="Y44" s="2"/>
     </row>
-    <row r="45" spans="1:25" ht="99.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:25" ht="105" x14ac:dyDescent="0.15">
       <c r="A45" s="4">
         <v>45</v>
       </c>
@@ -15755,7 +15748,7 @@
       <c r="X45" s="2"/>
       <c r="Y45" s="2"/>
     </row>
-    <row r="46" spans="1:25" ht="153.6" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:25" ht="153.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="4">
         <v>46</v>
       </c>
@@ -15806,7 +15799,7 @@
       <c r="X46" s="2"/>
       <c r="Y46" s="2"/>
     </row>
-    <row r="47" spans="1:25" ht="71.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:25" ht="75" x14ac:dyDescent="0.15">
       <c r="A47" s="4">
         <v>47</v>
       </c>
@@ -15859,7 +15852,7 @@
       <c r="X47" s="2"/>
       <c r="Y47" s="2"/>
     </row>
-    <row r="48" spans="1:25" ht="42.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:25" ht="45" x14ac:dyDescent="0.15">
       <c r="A48" s="4">
         <v>48</v>
       </c>
@@ -15912,7 +15905,7 @@
       <c r="X48" s="2"/>
       <c r="Y48" s="2"/>
     </row>
-    <row r="49" spans="1:25" ht="195.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:25" ht="195.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="4">
         <v>49</v>
       </c>
@@ -15977,7 +15970,7 @@
       <c r="X49" s="2"/>
       <c r="Y49" s="2"/>
     </row>
-    <row r="50" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A50" s="4">
         <v>50</v>
       </c>
@@ -16042,7 +16035,7 @@
       <c r="X50" s="2"/>
       <c r="Y50" s="2"/>
     </row>
-    <row r="51" spans="1:25" ht="340.35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:25" ht="340.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="4">
         <v>51</v>
       </c>
@@ -16093,7 +16086,7 @@
       <c r="X51" s="2"/>
       <c r="Y51" s="2"/>
     </row>
-    <row r="52" spans="1:25" ht="342" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:25" ht="356" x14ac:dyDescent="0.15">
       <c r="A52" s="4">
         <v>52</v>
       </c>
@@ -16152,7 +16145,7 @@
       <c r="X52" s="2"/>
       <c r="Y52" s="2"/>
     </row>
-    <row r="53" spans="1:25" ht="188.85" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:25" ht="188.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="4">
         <v>53</v>
       </c>
@@ -16221,7 +16214,7 @@
       <c r="X53" s="2"/>
       <c r="Y53" s="2"/>
     </row>
-    <row r="54" spans="1:25" ht="230.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:25" ht="230" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="4">
         <v>54</v>
       </c>
@@ -16288,7 +16281,7 @@
       <c r="X54" s="2"/>
       <c r="Y54" s="2"/>
     </row>
-    <row r="55" spans="1:25" ht="263.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:25" ht="263.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="4">
         <v>55</v>
       </c>
@@ -16345,7 +16338,7 @@
       <c r="X55" s="2"/>
       <c r="Y55" s="2"/>
     </row>
-    <row r="56" spans="1:25" ht="228" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:25" ht="255" x14ac:dyDescent="0.15">
       <c r="A56" s="4">
         <v>56</v>
       </c>
@@ -16410,7 +16403,7 @@
       <c r="X56" s="2"/>
       <c r="Y56" s="2"/>
     </row>
-    <row r="57" spans="1:25" ht="282" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:25" ht="282" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="4">
         <v>57</v>
       </c>
@@ -16477,7 +16470,7 @@
       <c r="X57" s="2"/>
       <c r="Y57" s="2"/>
     </row>
-    <row r="58" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A58" s="4">
         <v>58</v>
       </c>
@@ -16538,7 +16531,7 @@
       <c r="X58" s="2"/>
       <c r="Y58" s="2"/>
     </row>
-    <row r="59" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A59" s="4">
         <v>59</v>
       </c>
@@ -16603,7 +16596,7 @@
       <c r="X59" s="2"/>
       <c r="Y59" s="2"/>
     </row>
-    <row r="60" spans="1:25" ht="199.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:25" ht="210" x14ac:dyDescent="0.15">
       <c r="A60" s="4">
         <v>60</v>
       </c>
@@ -16644,7 +16637,7 @@
       <c r="X60" s="2"/>
       <c r="Y60" s="2"/>
     </row>
-    <row r="61" spans="1:25" ht="285" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:25" ht="300" x14ac:dyDescent="0.15">
       <c r="A61" s="4">
         <v>61</v>
       </c>
@@ -16691,7 +16684,7 @@
       <c r="X61" s="2"/>
       <c r="Y61" s="2"/>
     </row>
-    <row r="62" spans="1:25" ht="242.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:25" ht="270" x14ac:dyDescent="0.15">
       <c r="A62" s="4">
         <v>62</v>
       </c>
@@ -16750,7 +16743,7 @@
       <c r="X62" s="2"/>
       <c r="Y62" s="2"/>
     </row>
-    <row r="63" spans="1:25" ht="213.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:25" ht="225" x14ac:dyDescent="0.15">
       <c r="A63" s="4">
         <v>63</v>
       </c>
@@ -16809,7 +16802,7 @@
       <c r="X63" s="2"/>
       <c r="Y63" s="2"/>
     </row>
-    <row r="64" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A64" s="4">
         <v>64</v>
       </c>
@@ -16868,7 +16861,7 @@
       <c r="X64" s="2"/>
       <c r="Y64" s="2"/>
     </row>
-    <row r="65" spans="1:25" ht="254.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:25" ht="254" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="4">
         <v>65</v>
       </c>
@@ -16935,7 +16928,7 @@
       <c r="X65" s="2"/>
       <c r="Y65" s="2"/>
     </row>
-    <row r="66" spans="1:25" ht="85.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:25" ht="90" x14ac:dyDescent="0.15">
       <c r="A66" s="4">
         <v>66</v>
       </c>
@@ -16988,7 +16981,7 @@
       <c r="X66" s="2"/>
       <c r="Y66" s="2"/>
     </row>
-    <row r="67" spans="1:25" ht="384.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:25" ht="398" x14ac:dyDescent="0.15">
       <c r="A67" s="4">
         <v>67</v>
       </c>
@@ -17043,7 +17036,7 @@
       <c r="X67" s="2"/>
       <c r="Y67" s="2"/>
     </row>
-    <row r="68" spans="1:25" ht="254.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:25" ht="254.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="4">
         <v>68</v>
       </c>
@@ -17104,7 +17097,7 @@
       <c r="X68" s="2"/>
       <c r="Y68" s="2"/>
     </row>
-    <row r="69" spans="1:25" ht="384.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:25" ht="398" x14ac:dyDescent="0.15">
       <c r="A69" s="4">
         <v>69</v>
       </c>
@@ -17167,7 +17160,7 @@
       <c r="X69" s="2"/>
       <c r="Y69" s="2"/>
     </row>
-    <row r="70" spans="1:25" ht="142.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:25" ht="150" x14ac:dyDescent="0.15">
       <c r="A70" s="4">
         <v>70</v>
       </c>
@@ -17232,7 +17225,7 @@
       <c r="X70" s="2"/>
       <c r="Y70" s="2"/>
     </row>
-    <row r="71" spans="1:25" ht="85.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:25" ht="90" x14ac:dyDescent="0.15">
       <c r="A71" s="4">
         <v>71</v>
       </c>
@@ -17283,7 +17276,7 @@
       <c r="X71" s="2"/>
       <c r="Y71" s="2"/>
     </row>
-    <row r="72" spans="1:25" ht="269.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:25" ht="269.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="4">
         <v>72</v>
       </c>
@@ -17326,7 +17319,7 @@
       <c r="X72" s="2"/>
       <c r="Y72" s="2"/>
     </row>
-    <row r="73" spans="1:25" ht="242.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:25" ht="255" x14ac:dyDescent="0.15">
       <c r="A73" s="4">
         <v>73</v>
       </c>
@@ -17375,7 +17368,7 @@
       <c r="X73" s="2"/>
       <c r="Y73" s="2"/>
     </row>
-    <row r="74" spans="1:25" ht="231.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:25" ht="231.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="4">
         <v>74</v>
       </c>
@@ -17438,7 +17431,7 @@
       <c r="X74" s="2"/>
       <c r="Y74" s="2"/>
     </row>
-    <row r="75" spans="1:25" ht="347.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:25" ht="347.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="4">
         <v>75</v>
       </c>
@@ -17499,7 +17492,7 @@
       <c r="X75" s="2"/>
       <c r="Y75" s="2"/>
     </row>
-    <row r="76" spans="1:25" ht="294.60000000000002" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:25" ht="294.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="4">
         <v>76</v>
       </c>
@@ -17556,7 +17549,7 @@
       <c r="X76" s="2"/>
       <c r="Y76" s="2"/>
     </row>
-    <row r="77" spans="1:25" ht="409.6" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:25" ht="409.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="4">
         <v>77</v>
       </c>
@@ -17617,7 +17610,7 @@
       <c r="X77" s="2"/>
       <c r="Y77" s="2"/>
     </row>
-    <row r="78" spans="1:25" ht="331.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:25" ht="358" x14ac:dyDescent="0.15">
       <c r="A78" s="4">
         <v>78</v>
       </c>
@@ -17682,7 +17675,7 @@
       <c r="X78" s="2"/>
       <c r="Y78" s="2"/>
     </row>
-    <row r="79" spans="1:25" ht="271.35000000000002" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:25" ht="271.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="4">
         <v>79</v>
       </c>
@@ -17737,7 +17730,7 @@
       <c r="X79" s="2"/>
       <c r="Y79" s="2"/>
     </row>
-    <row r="80" spans="1:25" ht="270.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:25" ht="285" x14ac:dyDescent="0.15">
       <c r="A80" s="4">
         <v>80</v>
       </c>
@@ -17792,7 +17785,7 @@
       <c r="X80" s="2"/>
       <c r="Y80" s="2"/>
     </row>
-    <row r="81" spans="1:25" ht="270.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:25" ht="285" x14ac:dyDescent="0.15">
       <c r="A81" s="4">
         <v>81</v>
       </c>
@@ -17845,7 +17838,7 @@
       <c r="X81" s="2"/>
       <c r="Y81" s="2"/>
     </row>
-    <row r="82" spans="1:25" ht="270.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:25" ht="285" x14ac:dyDescent="0.15">
       <c r="A82" s="4">
         <v>82</v>
       </c>
@@ -17890,7 +17883,7 @@
       <c r="X82" s="2"/>
       <c r="Y82" s="2"/>
     </row>
-    <row r="83" spans="1:25" ht="180" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:25" ht="180" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="4">
         <v>83</v>
       </c>
@@ -17935,7 +17928,7 @@
       <c r="X83" s="2"/>
       <c r="Y83" s="2"/>
     </row>
-    <row r="84" spans="1:25" ht="192" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:25" ht="192" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="4">
         <v>84</v>
       </c>
@@ -17980,7 +17973,7 @@
       <c r="X84" s="2"/>
       <c r="Y84" s="2"/>
     </row>
-    <row r="85" spans="1:25" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:25" ht="120" x14ac:dyDescent="0.15">
       <c r="A85" s="4">
         <v>85</v>
       </c>
@@ -18025,7 +18018,7 @@
       <c r="X85" s="2"/>
       <c r="Y85" s="2"/>
     </row>
-    <row r="86" spans="1:25" ht="156.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:25" ht="165" x14ac:dyDescent="0.15">
       <c r="A86" s="4">
         <v>86</v>
       </c>
@@ -18076,7 +18069,7 @@
       <c r="X86" s="2"/>
       <c r="Y86" s="2"/>
     </row>
-    <row r="87" spans="1:25" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:25" ht="120" x14ac:dyDescent="0.15">
       <c r="A87" s="4">
         <v>87</v>
       </c>
@@ -18129,7 +18122,7 @@
       <c r="X87" s="2"/>
       <c r="Y87" s="2"/>
     </row>
-    <row r="88" spans="1:25" ht="185.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:25" ht="210" x14ac:dyDescent="0.15">
       <c r="A88" s="4">
         <v>88</v>
       </c>
@@ -18184,7 +18177,7 @@
       <c r="X88" s="2"/>
       <c r="Y88" s="2"/>
     </row>
-    <row r="89" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A89" s="4">
         <v>89</v>
       </c>
@@ -18241,7 +18234,7 @@
       <c r="X89" s="2"/>
       <c r="Y89" s="2"/>
     </row>
-    <row r="90" spans="1:25" ht="242.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:25" ht="285" x14ac:dyDescent="0.15">
       <c r="A90" s="4">
         <v>90</v>
       </c>
@@ -18288,7 +18281,7 @@
       <c r="X90" s="2"/>
       <c r="Y90" s="2"/>
     </row>
-    <row r="91" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A91" s="4">
         <v>91</v>
       </c>
@@ -18335,7 +18328,7 @@
       <c r="X91" s="2"/>
       <c r="Y91" s="2"/>
     </row>
-    <row r="92" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A92" s="4">
         <v>92</v>
       </c>
@@ -18382,7 +18375,7 @@
       <c r="X92" s="2"/>
       <c r="Y92" s="2"/>
     </row>
-    <row r="93" spans="1:25" ht="185.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:25" ht="195" x14ac:dyDescent="0.15">
       <c r="A93" s="4">
         <v>93</v>
       </c>
@@ -18435,7 +18428,7 @@
       <c r="X93" s="2"/>
       <c r="Y93" s="2"/>
     </row>
-    <row r="94" spans="1:25" ht="342" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:25" ht="356" x14ac:dyDescent="0.15">
       <c r="A94" s="4">
         <v>94</v>
       </c>
@@ -18490,7 +18483,7 @@
       <c r="X94" s="2"/>
       <c r="Y94" s="2"/>
     </row>
-    <row r="95" spans="1:25" ht="242.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:25" ht="255" x14ac:dyDescent="0.15">
       <c r="A95" s="4">
         <v>95</v>
       </c>
@@ -18545,7 +18538,7 @@
       <c r="X95" s="2"/>
       <c r="Y95" s="2"/>
     </row>
-    <row r="96" spans="1:25" ht="267.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:25" ht="267.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="4">
         <v>96</v>
       </c>
@@ -18598,7 +18591,7 @@
       <c r="X96" s="2"/>
       <c r="Y96" s="2"/>
     </row>
-    <row r="97" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A97" s="4">
         <v>97</v>
       </c>
@@ -18657,7 +18650,7 @@
       <c r="X97" s="2"/>
       <c r="Y97" s="2"/>
     </row>
-    <row r="98" spans="1:25" ht="213.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:25" ht="240" x14ac:dyDescent="0.15">
       <c r="A98" s="4">
         <v>98</v>
       </c>
@@ -18710,7 +18703,7 @@
       <c r="X98" s="2"/>
       <c r="Y98" s="2"/>
     </row>
-    <row r="99" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A99" s="4">
         <v>99</v>
       </c>
@@ -18769,7 +18762,7 @@
       <c r="X99" s="2"/>
       <c r="Y99" s="2"/>
     </row>
-    <row r="100" spans="1:25" ht="312.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:25" ht="312.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A100" s="4">
         <v>100</v>
       </c>
@@ -18818,7 +18811,7 @@
       <c r="X100" s="2"/>
       <c r="Y100" s="2"/>
     </row>
-    <row r="101" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A101" s="4">
         <v>101</v>
       </c>
@@ -18875,7 +18868,7 @@
       <c r="X101" s="2"/>
       <c r="Y101" s="2"/>
     </row>
-    <row r="102" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A102" s="4">
         <v>102</v>
       </c>
@@ -18932,7 +18925,7 @@
       <c r="X102" s="2"/>
       <c r="Y102" s="2"/>
     </row>
-    <row r="103" spans="1:25" ht="242.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:25" ht="270" x14ac:dyDescent="0.15">
       <c r="A103" s="4">
         <v>103</v>
       </c>
@@ -18991,7 +18984,7 @@
       <c r="X103" s="2"/>
       <c r="Y103" s="2"/>
     </row>
-    <row r="104" spans="1:25" ht="313.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:25" ht="342" x14ac:dyDescent="0.15">
       <c r="A104" s="4">
         <v>104</v>
       </c>
@@ -19050,7 +19043,7 @@
       <c r="X104" s="2"/>
       <c r="Y104" s="2"/>
     </row>
-    <row r="105" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A105" s="4">
         <v>105</v>
       </c>
@@ -19105,7 +19098,7 @@
       <c r="X105" s="2"/>
       <c r="Y105" s="2"/>
     </row>
-    <row r="106" spans="1:25" ht="256.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:25" ht="300" x14ac:dyDescent="0.15">
       <c r="A106" s="4">
         <v>106</v>
       </c>
@@ -19160,7 +19153,7 @@
       <c r="X106" s="2"/>
       <c r="Y106" s="2"/>
     </row>
-    <row r="107" spans="1:25" ht="128.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:25" ht="135" x14ac:dyDescent="0.15">
       <c r="A107" s="4">
         <v>107</v>
       </c>
@@ -19217,7 +19210,7 @@
       <c r="X107" s="2"/>
       <c r="Y107" s="2"/>
     </row>
-    <row r="108" spans="1:25" ht="85.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:25" ht="90" x14ac:dyDescent="0.15">
       <c r="A108" s="4">
         <v>108</v>
       </c>
@@ -19270,7 +19263,7 @@
       <c r="X108" s="2"/>
       <c r="Y108" s="2"/>
     </row>
-    <row r="109" spans="1:25" ht="228" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:25" ht="255" x14ac:dyDescent="0.15">
       <c r="A109" s="4">
         <v>109</v>
       </c>
@@ -19331,7 +19324,7 @@
       <c r="X109" s="2"/>
       <c r="Y109" s="2"/>
     </row>
-    <row r="110" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A110" s="4">
         <v>110</v>
       </c>
@@ -19390,7 +19383,7 @@
       <c r="X110" s="2"/>
       <c r="Y110" s="2"/>
     </row>
-    <row r="111" spans="1:25" ht="213.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:25" ht="225" x14ac:dyDescent="0.15">
       <c r="A111" s="4">
         <v>111</v>
       </c>
@@ -19437,7 +19430,7 @@
       <c r="X111" s="2"/>
       <c r="Y111" s="2"/>
     </row>
-    <row r="112" spans="1:25" ht="270.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:25" ht="300" x14ac:dyDescent="0.15">
       <c r="A112" s="4">
         <v>112</v>
       </c>
@@ -19484,7 +19477,7 @@
       <c r="X112" s="2"/>
       <c r="Y112" s="2"/>
     </row>
-    <row r="113" spans="1:25" ht="253.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:25" ht="253.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A113" s="4">
         <v>113</v>
       </c>
@@ -19541,7 +19534,7 @@
       <c r="X113" s="2"/>
       <c r="Y113" s="2"/>
     </row>
-    <row r="114" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A114" s="4">
         <v>114</v>
       </c>
@@ -19604,7 +19597,7 @@
       <c r="X114" s="2"/>
       <c r="Y114" s="2"/>
     </row>
-    <row r="115" spans="1:25" ht="98.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:25" ht="98" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A115" s="4">
         <v>115</v>
       </c>
@@ -19661,7 +19654,7 @@
       <c r="X115" s="2"/>
       <c r="Y115" s="2"/>
     </row>
-    <row r="116" spans="1:25" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A116" s="4">
         <v>116</v>
       </c>
@@ -19716,7 +19709,7 @@
       <c r="X116" s="2"/>
       <c r="Y116" s="2"/>
     </row>
-    <row r="117" spans="1:25" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A117" s="4">
         <v>117</v>
       </c>
@@ -19771,7 +19764,7 @@
       <c r="X117" s="2"/>
       <c r="Y117" s="2"/>
     </row>
-    <row r="118" spans="1:25" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:25" ht="60" x14ac:dyDescent="0.15">
       <c r="A118" s="4">
         <v>118</v>
       </c>
@@ -19824,7 +19817,7 @@
       <c r="X118" s="2"/>
       <c r="Y118" s="2"/>
     </row>
-    <row r="119" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A119" s="4">
         <v>119</v>
       </c>
@@ -19883,7 +19876,7 @@
       <c r="X119" s="2"/>
       <c r="Y119" s="2"/>
     </row>
-    <row r="120" spans="1:25" ht="327.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:25" ht="342" x14ac:dyDescent="0.15">
       <c r="A120" s="4">
         <v>120</v>
       </c>
@@ -19940,7 +19933,7 @@
       <c r="X120" s="2"/>
       <c r="Y120" s="2"/>
     </row>
-    <row r="121" spans="1:25" ht="244.35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:25" ht="244.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A121" s="4">
         <v>121</v>
       </c>
@@ -19995,7 +19988,7 @@
       <c r="X121" s="2"/>
       <c r="Y121" s="2"/>
     </row>
-    <row r="122" spans="1:25" ht="270.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:25" ht="285" x14ac:dyDescent="0.15">
       <c r="A122" s="4">
         <v>122</v>
       </c>
@@ -20048,7 +20041,7 @@
       <c r="X122" s="2"/>
       <c r="Y122" s="2"/>
     </row>
-    <row r="123" spans="1:25" ht="189" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:25" ht="189" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="4">
         <v>123</v>
       </c>
@@ -20095,7 +20088,7 @@
       <c r="X123" s="2"/>
       <c r="Y123" s="2"/>
     </row>
-    <row r="124" spans="1:25" ht="327.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:25" ht="342" x14ac:dyDescent="0.2">
       <c r="A124" s="4">
         <v>124</v>
       </c>
@@ -20148,7 +20141,7 @@
       <c r="X124" s="2"/>
       <c r="Y124" s="2"/>
     </row>
-    <row r="125" spans="1:25" ht="285" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:25" ht="300" x14ac:dyDescent="0.2">
       <c r="A125" s="4">
         <v>125</v>
       </c>
@@ -20201,7 +20194,7 @@
       <c r="X125" s="2"/>
       <c r="Y125" s="2"/>
     </row>
-    <row r="126" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A126" s="4">
         <v>126</v>
       </c>
@@ -20260,7 +20253,7 @@
       <c r="X126" s="2"/>
       <c r="Y126" s="2"/>
     </row>
-    <row r="127" spans="1:25" ht="242.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:25" ht="255" x14ac:dyDescent="0.15">
       <c r="A127" s="4">
         <v>127</v>
       </c>
@@ -20300,7 +20293,7 @@
       <c r="X127" s="2"/>
       <c r="Y127" s="2"/>
     </row>
-    <row r="128" spans="1:25" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:25" ht="120" x14ac:dyDescent="0.15">
       <c r="A128" s="4">
         <v>128</v>
       </c>
@@ -20345,7 +20338,7 @@
       <c r="X128" s="2"/>
       <c r="Y128" s="2"/>
     </row>
-    <row r="129" spans="1:25" ht="213.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:25" ht="225" x14ac:dyDescent="0.15">
       <c r="A129" s="4">
         <v>129</v>
       </c>
@@ -20406,7 +20399,7 @@
       <c r="X129" s="2"/>
       <c r="Y129" s="2"/>
     </row>
-    <row r="130" spans="1:25" ht="256.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:25" ht="270" x14ac:dyDescent="0.15">
       <c r="A130" s="4">
         <v>130</v>
       </c>
@@ -20463,7 +20456,7 @@
       <c r="X130" s="2"/>
       <c r="Y130" s="2"/>
     </row>
-    <row r="131" spans="1:25" ht="343.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:25" ht="370" x14ac:dyDescent="0.15">
       <c r="A131" s="4">
         <v>131</v>
       </c>
@@ -20524,7 +20517,7 @@
       <c r="X131" s="2"/>
       <c r="Y131" s="2"/>
     </row>
-    <row r="132" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A132" s="4">
         <v>132</v>
       </c>
@@ -20573,7 +20566,7 @@
       <c r="X132" s="2"/>
       <c r="Y132" s="2"/>
     </row>
-    <row r="133" spans="1:25" ht="142.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:25" ht="150" x14ac:dyDescent="0.15">
       <c r="A133" s="4">
         <v>133</v>
       </c>
@@ -20616,7 +20609,7 @@
       <c r="X133" s="2"/>
       <c r="Y133" s="2"/>
     </row>
-    <row r="134" spans="1:25" ht="327.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:25" ht="342" x14ac:dyDescent="0.15">
       <c r="A134" s="4">
         <v>134</v>
       </c>
@@ -20669,7 +20662,7 @@
       <c r="X134" s="2"/>
       <c r="Y134" s="2"/>
     </row>
-    <row r="135" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A135" s="4">
         <v>135</v>
       </c>
@@ -20718,7 +20711,7 @@
       <c r="X135" s="2"/>
       <c r="Y135" s="2"/>
     </row>
-    <row r="136" spans="1:25" ht="351" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:25" ht="351" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A136" s="4">
         <v>136</v>
       </c>
@@ -20771,7 +20764,7 @@
       <c r="X136" s="2"/>
       <c r="Y136" s="2"/>
     </row>
-    <row r="137" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A137" s="4">
         <v>137</v>
       </c>
@@ -20828,7 +20821,7 @@
       <c r="X137" s="2"/>
       <c r="Y137" s="2"/>
     </row>
-    <row r="138" spans="1:25" ht="185.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:25" ht="210" x14ac:dyDescent="0.15">
       <c r="A138" s="4">
         <v>138</v>
       </c>
@@ -20889,7 +20882,7 @@
       <c r="X138" s="2"/>
       <c r="Y138" s="2"/>
     </row>
-    <row r="139" spans="1:25" ht="156.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:25" ht="180" x14ac:dyDescent="0.15">
       <c r="A139" s="4">
         <v>139</v>
       </c>
@@ -20948,7 +20941,7 @@
       <c r="X139" s="2"/>
       <c r="Y139" s="2"/>
     </row>
-    <row r="140" spans="1:25" ht="178.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:25" ht="178.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A140" s="4">
         <v>140</v>
       </c>
@@ -21003,7 +20996,7 @@
       <c r="X140" s="2"/>
       <c r="Y140" s="2"/>
     </row>
-    <row r="141" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A141" s="4">
         <v>141</v>
       </c>
@@ -21066,7 +21059,7 @@
       <c r="X141" s="2"/>
       <c r="Y141" s="2"/>
     </row>
-    <row r="142" spans="1:25" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:25" ht="409.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A142" s="4">
         <v>142</v>
       </c>
@@ -21129,7 +21122,7 @@
       <c r="X142" s="2"/>
       <c r="Y142" s="2"/>
     </row>
-    <row r="143" spans="1:25" ht="142.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:25" ht="150" x14ac:dyDescent="0.15">
       <c r="A143" s="4">
         <v>143</v>
       </c>
@@ -21186,7 +21179,7 @@
       <c r="X143" s="2"/>
       <c r="Y143" s="2"/>
     </row>
-    <row r="144" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A144" s="4">
         <v>144</v>
       </c>
@@ -21247,7 +21240,7 @@
       <c r="X144" s="2"/>
       <c r="Y144" s="2"/>
     </row>
-    <row r="145" spans="1:25" ht="332.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:25" ht="332" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A145" s="4">
         <v>145</v>
       </c>
@@ -21306,7 +21299,7 @@
       <c r="X145" s="2"/>
       <c r="Y145" s="2"/>
     </row>
-    <row r="146" spans="1:25" ht="278.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:25" ht="278.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A146" s="4">
         <v>146</v>
       </c>
@@ -21355,7 +21348,7 @@
       <c r="X146" s="2"/>
       <c r="Y146" s="2"/>
     </row>
-    <row r="147" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A147" s="4">
         <v>147</v>
       </c>
@@ -21402,7 +21395,7 @@
       <c r="X147" s="2"/>
       <c r="Y147" s="2"/>
     </row>
-    <row r="148" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A148" s="4">
         <v>148</v>
       </c>
@@ -21463,7 +21456,7 @@
       <c r="X148" s="2"/>
       <c r="Y148" s="2"/>
     </row>
-    <row r="149" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A149" s="4">
         <v>149</v>
       </c>
@@ -21516,7 +21509,7 @@
       <c r="X149" s="2"/>
       <c r="Y149" s="2"/>
     </row>
-    <row r="150" spans="1:25" ht="201" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:25" ht="201" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A150" s="4">
         <v>150</v>
       </c>
@@ -21573,7 +21566,7 @@
       <c r="X150" s="2"/>
       <c r="Y150" s="2"/>
     </row>
-    <row r="151" spans="1:25" ht="201" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:25" ht="201" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A151" s="4">
         <v>151</v>
       </c>
@@ -21620,7 +21613,7 @@
       <c r="X151" s="2"/>
       <c r="Y151" s="2"/>
     </row>
-    <row r="152" spans="1:25" ht="228" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:25" ht="240" x14ac:dyDescent="0.15">
       <c r="A152" s="4">
         <v>152</v>
       </c>
@@ -21671,7 +21664,7 @@
       <c r="X152" s="2"/>
       <c r="Y152" s="2"/>
     </row>
-    <row r="153" spans="1:25" ht="342" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:25" ht="356" x14ac:dyDescent="0.15">
       <c r="A153" s="4">
         <v>153</v>
       </c>
@@ -21724,7 +21717,7 @@
       <c r="X153" s="2"/>
       <c r="Y153" s="2"/>
     </row>
-    <row r="154" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A154" s="4">
         <v>154</v>
       </c>
@@ -21773,7 +21766,7 @@
       <c r="X154" s="2"/>
       <c r="Y154" s="2"/>
     </row>
-    <row r="155" spans="1:25" ht="71.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:25" ht="75" x14ac:dyDescent="0.15">
       <c r="A155" s="4">
         <v>155</v>
       </c>
@@ -21828,7 +21821,7 @@
       <c r="X155" s="2"/>
       <c r="Y155" s="2"/>
     </row>
-    <row r="156" spans="1:25" ht="399" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A156" s="4">
         <v>156</v>
       </c>
@@ -21890,7 +21883,7 @@
       <c r="X156" s="2"/>
       <c r="Y156" s="2"/>
     </row>
-    <row r="157" spans="1:25" ht="299.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:25" ht="314" x14ac:dyDescent="0.15">
       <c r="A157" s="4">
         <v>157</v>
       </c>
@@ -21937,7 +21930,7 @@
       <c r="X157" s="2"/>
       <c r="Y157" s="2"/>
     </row>
-    <row r="158" spans="1:25" ht="156.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:25" ht="180" x14ac:dyDescent="0.15">
       <c r="A158" s="4">
         <v>158</v>
       </c>
@@ -21986,7 +21979,7 @@
       <c r="X158" s="2"/>
       <c r="Y158" s="2"/>
     </row>
-    <row r="159" spans="1:25" ht="370.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:25" ht="398" x14ac:dyDescent="0.15">
       <c r="A159" s="4">
         <v>159</v>
       </c>
@@ -22047,7 +22040,7 @@
       <c r="X159" s="2"/>
       <c r="Y159" s="2"/>
     </row>
-    <row r="160" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A160" s="4">
         <v>160</v>
       </c>
@@ -22108,7 +22101,7 @@
       <c r="X160" s="2"/>
       <c r="Y160" s="2"/>
     </row>
-    <row r="161" spans="1:25" ht="156.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:25" ht="165" x14ac:dyDescent="0.15">
       <c r="A161" s="4">
         <v>161</v>
       </c>
@@ -22155,7 +22148,7 @@
       <c r="X161" s="2"/>
       <c r="Y161" s="2"/>
     </row>
-    <row r="162" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A162" s="4">
         <v>162</v>
       </c>
@@ -22212,7 +22205,7 @@
       <c r="X162" s="2"/>
       <c r="Y162" s="2"/>
     </row>
-    <row r="163" spans="1:25" ht="351.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:25" ht="351.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A163" s="4">
         <v>163</v>
       </c>
@@ -22271,7 +22264,7 @@
       <c r="X163" s="2"/>
       <c r="Y163" s="2"/>
     </row>
-    <row r="164" spans="1:25" ht="303.60000000000002" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:25" ht="303.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A164" s="4">
         <v>164</v>
       </c>
@@ -22330,7 +22323,7 @@
       <c r="X164" s="2"/>
       <c r="Y164" s="2"/>
     </row>
-    <row r="165" spans="1:25" ht="99.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:25" ht="105" x14ac:dyDescent="0.15">
       <c r="A165" s="4">
         <v>165</v>
       </c>
@@ -22381,7 +22374,7 @@
       <c r="X165" s="2"/>
       <c r="Y165" s="2"/>
     </row>
-    <row r="166" spans="1:25" ht="285" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:25" ht="314" x14ac:dyDescent="0.15">
       <c r="A166" s="4">
         <v>166</v>
       </c>
@@ -22432,7 +22425,7 @@
       <c r="X166" s="2"/>
       <c r="Y166" s="2"/>
     </row>
-    <row r="167" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A167" s="4">
         <v>167</v>
       </c>
@@ -22489,7 +22482,7 @@
       <c r="X167" s="2"/>
       <c r="Y167" s="2"/>
     </row>
-    <row r="168" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A168" s="4">
         <v>168</v>
       </c>
@@ -22550,7 +22543,7 @@
       <c r="X168" s="2"/>
       <c r="Y168" s="2"/>
     </row>
-    <row r="169" spans="1:25" ht="270.75" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:25" ht="300" x14ac:dyDescent="0.15">
       <c r="A169" s="4">
         <v>169</v>
       </c>
@@ -22603,7 +22596,7 @@
       <c r="X169" s="2"/>
       <c r="Y169" s="2"/>
     </row>
-    <row r="170" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A170" s="4">
         <v>170</v>
       </c>
@@ -22646,7 +22639,7 @@
       <c r="X170" s="2"/>
       <c r="Y170" s="2"/>
     </row>
-    <row r="171" spans="1:25" ht="71.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:25" ht="75" x14ac:dyDescent="0.15">
       <c r="A171" s="4">
         <v>171</v>
       </c>
@@ -22689,7 +22682,7 @@
       <c r="X171" s="2"/>
       <c r="Y171" s="2"/>
     </row>
-    <row r="172" spans="1:25" ht="299.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:25" ht="314" x14ac:dyDescent="0.15">
       <c r="A172" s="4">
         <v>172</v>
       </c>
@@ -22740,7 +22733,7 @@
       <c r="X172" s="2"/>
       <c r="Y172" s="2"/>
     </row>
-    <row r="173" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A173" s="4">
         <v>173</v>
       </c>
@@ -22787,7 +22780,7 @@
       <c r="X173" s="2"/>
       <c r="Y173" s="2"/>
     </row>
-    <row r="174" spans="1:25" ht="384.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:25" ht="398" x14ac:dyDescent="0.15">
       <c r="A174" s="4">
         <v>174</v>
       </c>
@@ -22828,7 +22821,7 @@
       <c r="X174" s="2"/>
       <c r="Y174" s="2"/>
     </row>
-    <row r="175" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A175" s="4">
         <v>175</v>
       </c>
@@ -22879,7 +22872,7 @@
       <c r="X175" s="2"/>
       <c r="Y175" s="2"/>
     </row>
-    <row r="176" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A176" s="4">
         <v>176</v>
       </c>
@@ -22944,7 +22937,7 @@
       <c r="X176" s="2"/>
       <c r="Y176" s="2"/>
     </row>
-    <row r="177" spans="1:25" ht="164.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:25" ht="164" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A177" s="4">
         <v>177</v>
       </c>
@@ -23001,7 +22994,7 @@
       <c r="X177" s="2"/>
       <c r="Y177" s="2"/>
     </row>
-    <row r="178" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A178" s="4">
         <v>178</v>
       </c>
@@ -23060,7 +23053,7 @@
       <c r="X178" s="2"/>
       <c r="Y178" s="2"/>
     </row>
-    <row r="179" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A179" s="4">
         <v>179</v>
       </c>
@@ -23109,7 +23102,7 @@
       <c r="X179" s="2"/>
       <c r="Y179" s="2"/>
     </row>
-    <row r="180" spans="1:25" ht="199.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:25" ht="210" x14ac:dyDescent="0.15">
       <c r="A180" s="4">
         <v>180</v>
       </c>
@@ -23154,7 +23147,7 @@
       <c r="X180" s="2"/>
       <c r="Y180" s="2"/>
     </row>
-    <row r="181" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A181" s="4">
         <v>181</v>
       </c>
@@ -23199,7 +23192,7 @@
       <c r="X181" s="2"/>
       <c r="Y181" s="2"/>
     </row>
-    <row r="182" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A182" s="4">
         <v>182</v>
       </c>
@@ -23260,7 +23253,7 @@
       <c r="X182" s="2"/>
       <c r="Y182" s="2"/>
     </row>
-    <row r="183" spans="1:25" ht="309.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:25" ht="309.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A183" s="4">
         <v>183</v>
       </c>
@@ -23321,7 +23314,7 @@
       <c r="X183" s="2"/>
       <c r="Y183" s="2"/>
     </row>
-    <row r="184" spans="1:25" ht="227.85" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:25" ht="227.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A184" s="4">
         <v>184</v>
       </c>
@@ -23380,7 +23373,7 @@
       <c r="X184" s="2"/>
       <c r="Y184" s="2"/>
     </row>
-    <row r="185" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A185" s="4">
         <v>185</v>
       </c>
@@ -23423,7 +23416,7 @@
       <c r="X185" s="2"/>
       <c r="Y185" s="2"/>
     </row>
-    <row r="186" spans="1:25" ht="342" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:25" ht="356" x14ac:dyDescent="0.15">
       <c r="A186" s="4">
         <v>186</v>
       </c>
@@ -23480,7 +23473,7 @@
       <c r="X186" s="2"/>
       <c r="Y186" s="2"/>
     </row>
-    <row r="187" spans="1:25" ht="228" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:25" ht="240" x14ac:dyDescent="0.15">
       <c r="A187" s="4">
         <v>187</v>
       </c>
@@ -23523,7 +23516,7 @@
       <c r="X187" s="2"/>
       <c r="Y187" s="2"/>
     </row>
-    <row r="188" spans="1:25" ht="299.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:25" ht="314" x14ac:dyDescent="0.15">
       <c r="A188" s="4">
         <v>188</v>
       </c>
@@ -23566,7 +23559,7 @@
       <c r="X188" s="2"/>
       <c r="Y188" s="2"/>
     </row>
-    <row r="189" spans="1:25" ht="156.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:25" ht="180" x14ac:dyDescent="0.15">
       <c r="A189" s="4">
         <v>189</v>
       </c>
@@ -23615,7 +23608,7 @@
       <c r="X189" s="2"/>
       <c r="Y189" s="2"/>
     </row>
-    <row r="190" spans="1:25" ht="171" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:25" ht="180" x14ac:dyDescent="0.15">
       <c r="A190" s="4">
         <v>190</v>
       </c>
@@ -23658,7 +23651,7 @@
       <c r="X190" s="2"/>
       <c r="Y190" s="2"/>
     </row>
-    <row r="191" spans="1:25" ht="199.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:25" ht="210" x14ac:dyDescent="0.15">
       <c r="A191" s="4">
         <v>191</v>
       </c>
@@ -23701,7 +23694,7 @@
       <c r="X191" s="2"/>
       <c r="Y191" s="2"/>
     </row>
-    <row r="192" spans="1:25" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A192" s="4">
         <v>192</v>
       </c>
@@ -23758,7 +23751,7 @@
       <c r="X192" s="2"/>
       <c r="Y192" s="2"/>
     </row>
-    <row r="193" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A193" s="4">
         <v>193</v>
       </c>
@@ -23811,7 +23804,7 @@
       <c r="X193" s="2"/>
       <c r="Y193" s="2"/>
     </row>
-    <row r="194" spans="1:25" ht="370.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:25" ht="384" x14ac:dyDescent="0.15">
       <c r="A194" s="4">
         <v>194</v>
       </c>
@@ -23874,7 +23867,7 @@
       <c r="X194" s="2"/>
       <c r="Y194" s="2"/>
     </row>
-    <row r="195" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A195" s="4">
         <v>195</v>
       </c>
@@ -23917,7 +23910,7 @@
       <c r="X195" s="2"/>
       <c r="Y195" s="2"/>
     </row>
-    <row r="196" spans="1:25" ht="128.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:25" ht="135" x14ac:dyDescent="0.15">
       <c r="A196" s="4">
         <v>196</v>
       </c>
@@ -23960,7 +23953,7 @@
       <c r="X196" s="2"/>
       <c r="Y196" s="2"/>
     </row>
-    <row r="197" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A197" s="4">
         <v>197</v>
       </c>
@@ -24015,7 +24008,7 @@
       <c r="X197" s="2"/>
       <c r="Y197" s="2"/>
     </row>
-    <row r="198" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A198" s="4">
         <v>198</v>
       </c>
@@ -24066,7 +24059,7 @@
       <c r="X198" s="2"/>
       <c r="Y198" s="2"/>
     </row>
-    <row r="199" spans="1:25" ht="228" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:25" ht="240" x14ac:dyDescent="0.15">
       <c r="A199" s="4">
         <v>199</v>
       </c>
@@ -24117,7 +24110,7 @@
       <c r="X199" s="2"/>
       <c r="Y199" s="2"/>
     </row>
-    <row r="200" spans="1:25" ht="256.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:25" ht="270" x14ac:dyDescent="0.15">
       <c r="A200" s="4">
         <v>200</v>
       </c>
@@ -24174,7 +24167,7 @@
       <c r="X200" s="2"/>
       <c r="Y200" s="2"/>
     </row>
-    <row r="201" spans="1:25" ht="162.6" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:25" ht="162.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A201" s="4">
         <v>201</v>
       </c>
@@ -24231,7 +24224,7 @@
       <c r="X201" s="2"/>
       <c r="Y201" s="2"/>
     </row>
-    <row r="202" spans="1:25" ht="185.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:25" ht="195" x14ac:dyDescent="0.15">
       <c r="A202" s="4">
         <v>202</v>
       </c>
@@ -24290,7 +24283,7 @@
       <c r="X202" s="2"/>
       <c r="Y202" s="2"/>
     </row>
-    <row r="203" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A203" s="4">
         <v>203</v>
       </c>
@@ -24341,7 +24334,7 @@
       <c r="X203" s="2"/>
       <c r="Y203" s="2"/>
     </row>
-    <row r="204" spans="1:25" ht="407.85" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:25" ht="407.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A204" s="4">
         <v>204</v>
       </c>
@@ -24386,7 +24379,7 @@
       <c r="X204" s="2"/>
       <c r="Y204" s="2"/>
     </row>
-    <row r="205" spans="1:25" ht="324" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:25" ht="324" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A205" s="4">
         <v>205</v>
       </c>
@@ -24435,7 +24428,7 @@
       <c r="X205" s="2"/>
       <c r="Y205" s="2"/>
     </row>
-    <row r="206" spans="1:25" ht="219.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:25" ht="219.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A206" s="4">
         <v>206</v>
       </c>
@@ -24492,7 +24485,7 @@
       <c r="X206" s="2"/>
       <c r="Y206" s="2"/>
     </row>
-    <row r="207" spans="1:25" ht="256.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:25" ht="270" x14ac:dyDescent="0.15">
       <c r="A207" s="4">
         <v>207</v>
       </c>
@@ -24541,7 +24534,7 @@
       <c r="X207" s="2"/>
       <c r="Y207" s="2"/>
     </row>
-    <row r="208" spans="1:25" ht="370.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:25" ht="384" x14ac:dyDescent="0.15">
       <c r="A208" s="4">
         <v>208</v>
       </c>
@@ -24584,7 +24577,7 @@
       <c r="X208" s="2"/>
       <c r="Y208" s="2"/>
     </row>
-    <row r="209" spans="1:25" ht="201" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:25" ht="201" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A209" s="4">
         <v>209</v>
       </c>
@@ -24627,7 +24620,7 @@
       <c r="X209" s="2"/>
       <c r="Y209" s="2"/>
     </row>
-    <row r="210" spans="1:25" ht="85.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:25" ht="90" x14ac:dyDescent="0.15">
       <c r="A210" s="4">
         <v>210</v>
       </c>
@@ -24672,7 +24665,7 @@
       <c r="X210" s="2"/>
       <c r="Y210" s="2"/>
     </row>
-    <row r="211" spans="1:25" ht="356.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:25" ht="370" x14ac:dyDescent="0.15">
       <c r="A211" s="4">
         <v>211</v>
       </c>
@@ -24729,7 +24722,7 @@
       <c r="X211" s="2"/>
       <c r="Y211" s="2"/>
     </row>
-    <row r="212" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A212" s="4">
         <v>212</v>
       </c>
@@ -24772,7 +24765,7 @@
       <c r="X212" s="2"/>
       <c r="Y212" s="2"/>
     </row>
-    <row r="213" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A213" s="4">
         <v>213</v>
       </c>
@@ -24817,7 +24810,7 @@
       <c r="X213" s="2"/>
       <c r="Y213" s="2"/>
     </row>
-    <row r="214" spans="1:25" ht="71.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:25" ht="75" x14ac:dyDescent="0.15">
       <c r="A214" s="4">
         <v>214</v>
       </c>
@@ -24866,7 +24859,7 @@
       <c r="X214" s="2"/>
       <c r="Y214" s="2"/>
     </row>
-    <row r="215" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A215" s="4">
         <v>215</v>
       </c>
@@ -24909,7 +24902,7 @@
       <c r="X215" s="2"/>
       <c r="Y215" s="2"/>
     </row>
-    <row r="216" spans="1:25" ht="185.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:25" ht="195" x14ac:dyDescent="0.15">
       <c r="A216" s="4">
         <v>216</v>
       </c>
@@ -24966,7 +24959,7 @@
       <c r="X216" s="2"/>
       <c r="Y216" s="2"/>
     </row>
-    <row r="217" spans="1:25" ht="87" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:25" ht="87" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A217" s="4">
         <v>217</v>
       </c>
@@ -25009,7 +25002,7 @@
       <c r="X217" s="2"/>
       <c r="Y217" s="2"/>
     </row>
-    <row r="218" spans="1:25" ht="185.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:25" ht="195" x14ac:dyDescent="0.15">
       <c r="A218" s="4">
         <v>218</v>
       </c>
@@ -25052,7 +25045,7 @@
       <c r="X218" s="2"/>
       <c r="Y218" s="2"/>
     </row>
-    <row r="219" spans="1:25" ht="199.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:25" ht="210" x14ac:dyDescent="0.15">
       <c r="A219" s="4">
         <v>219</v>
       </c>
@@ -25095,7 +25088,7 @@
       <c r="X219" s="2"/>
       <c r="Y219" s="2"/>
     </row>
-    <row r="220" spans="1:25" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:25" ht="60" x14ac:dyDescent="0.15">
       <c r="A220" s="4">
         <v>220</v>
       </c>
@@ -25138,7 +25131,7 @@
       <c r="X220" s="2"/>
       <c r="Y220" s="2"/>
     </row>
-    <row r="221" spans="1:25" ht="156.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:25" ht="165" x14ac:dyDescent="0.15">
       <c r="A221" s="4">
         <v>221</v>
       </c>
@@ -25181,7 +25174,7 @@
       <c r="X221" s="2"/>
       <c r="Y221" s="2"/>
     </row>
-    <row r="222" spans="1:25" ht="285" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:25" ht="300" x14ac:dyDescent="0.15">
       <c r="A222" s="4">
         <v>222</v>
       </c>
@@ -25224,7 +25217,7 @@
       <c r="X222" s="2"/>
       <c r="Y222" s="2"/>
     </row>
-    <row r="223" spans="1:25" ht="128.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:25" ht="135" x14ac:dyDescent="0.15">
       <c r="A223" s="4">
         <v>223</v>
       </c>
@@ -25267,7 +25260,7 @@
       <c r="X223" s="2"/>
       <c r="Y223" s="2"/>
     </row>
-    <row r="224" spans="1:25" ht="71.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:25" ht="75" x14ac:dyDescent="0.15">
       <c r="A224" s="4">
         <v>224</v>
       </c>
@@ -25310,7 +25303,7 @@
       <c r="X224" s="2"/>
       <c r="Y224" s="2"/>
     </row>
-    <row r="225" spans="1:25" ht="42.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:25" ht="45" x14ac:dyDescent="0.15">
       <c r="A225" s="4">
         <v>225</v>
       </c>
@@ -25353,7 +25346,7 @@
       <c r="X225" s="2"/>
       <c r="Y225" s="2"/>
     </row>
-    <row r="226" spans="1:25" ht="128.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:25" ht="135" x14ac:dyDescent="0.15">
       <c r="A226" s="4">
         <v>226</v>
       </c>
@@ -25396,7 +25389,7 @@
       <c r="X226" s="2"/>
       <c r="Y226" s="2"/>
     </row>
-    <row r="227" spans="1:25" ht="28.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:25" ht="30" x14ac:dyDescent="0.15">
       <c r="A227" s="4">
         <v>227</v>
       </c>
@@ -25439,7 +25432,7 @@
       <c r="X227" s="2"/>
       <c r="Y227" s="2"/>
     </row>
-    <row r="228" spans="1:25" ht="171" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:25" ht="180" x14ac:dyDescent="0.15">
       <c r="A228" s="4">
         <v>228</v>
       </c>
@@ -25478,7 +25471,7 @@
       <c r="X228" s="2"/>
       <c r="Y228" s="2"/>
     </row>
-    <row r="229" spans="1:25" ht="86.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:25" ht="86.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A229" s="4">
         <v>229</v>
       </c>
@@ -25521,7 +25514,7 @@
       <c r="X229" s="2"/>
       <c r="Y229" s="2"/>
     </row>
-    <row r="230" spans="1:25" ht="356.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:25" ht="384" x14ac:dyDescent="0.15">
       <c r="A230" s="4">
         <v>230</v>
       </c>
@@ -25564,7 +25557,7 @@
       <c r="X230" s="2"/>
       <c r="Y230" s="2"/>
     </row>
-    <row r="231" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A231" s="4">
         <v>231</v>
       </c>
@@ -25607,7 +25600,7 @@
       <c r="X231" s="2"/>
       <c r="Y231" s="2"/>
     </row>
-    <row r="232" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A232" s="4">
         <v>232</v>
       </c>
@@ -25650,7 +25643,7 @@
       <c r="X232" s="2"/>
       <c r="Y232" s="2"/>
     </row>
-    <row r="233" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A233" s="4">
         <v>233</v>
       </c>
@@ -25693,7 +25686,7 @@
       <c r="X233" s="2"/>
       <c r="Y233" s="2"/>
     </row>
-    <row r="234" spans="1:25" ht="256.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:25" ht="270" x14ac:dyDescent="0.15">
       <c r="A234" s="4">
         <v>234</v>
       </c>
@@ -25740,7 +25733,7 @@
       <c r="X234" s="2"/>
       <c r="Y234" s="2"/>
     </row>
-    <row r="235" spans="1:25" ht="280.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:25" ht="280.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A235" s="4">
         <v>235</v>
       </c>
@@ -25783,7 +25776,7 @@
       <c r="X235" s="2"/>
       <c r="Y235" s="2"/>
     </row>
-    <row r="236" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A236" s="4">
         <v>236</v>
       </c>
@@ -25826,7 +25819,7 @@
       <c r="X236" s="2"/>
       <c r="Y236" s="2"/>
     </row>
-    <row r="237" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A237" s="4">
         <v>237</v>
       </c>
@@ -25871,7 +25864,7 @@
       <c r="X237" s="2"/>
       <c r="Y237" s="2"/>
     </row>
-    <row r="238" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A238" s="4">
         <v>238</v>
       </c>
@@ -25924,7 +25917,7 @@
       <c r="X238" s="2"/>
       <c r="Y238" s="2"/>
     </row>
-    <row r="239" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A239" s="4">
         <v>239</v>
       </c>
@@ -25967,7 +25960,7 @@
       <c r="X239" s="2"/>
       <c r="Y239" s="2"/>
     </row>
-    <row r="240" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A240" s="4">
         <v>240</v>
       </c>
@@ -26010,7 +26003,7 @@
       <c r="X240" s="2"/>
       <c r="Y240" s="2"/>
     </row>
-    <row r="241" spans="1:25" ht="57" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:25" ht="75" x14ac:dyDescent="0.15">
       <c r="A241" s="4">
         <v>241</v>
       </c>
@@ -26053,7 +26046,7 @@
       <c r="X241" s="2"/>
       <c r="Y241" s="2"/>
     </row>
-    <row r="242" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A242" s="4">
         <v>242</v>
       </c>
@@ -26096,7 +26089,7 @@
       <c r="X242" s="2"/>
       <c r="Y242" s="2"/>
     </row>
-    <row r="243" spans="1:25" ht="199.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:25" ht="210" x14ac:dyDescent="0.15">
       <c r="A243" s="4">
         <v>243</v>
       </c>
@@ -26141,7 +26134,7 @@
       <c r="X243" s="2"/>
       <c r="Y243" s="2"/>
     </row>
-    <row r="244" spans="1:25" ht="152.85" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:25" ht="152.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A244" s="4">
         <v>244</v>
       </c>
@@ -26186,7 +26179,7 @@
       <c r="X244" s="2"/>
       <c r="Y244" s="2"/>
     </row>
-    <row r="245" spans="1:25" ht="370.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:25" ht="384" x14ac:dyDescent="0.15">
       <c r="A245" s="4">
         <v>245</v>
       </c>
@@ -26231,7 +26224,7 @@
       <c r="X245" s="2"/>
       <c r="Y245" s="2"/>
     </row>
-    <row r="246" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A246" s="4">
         <v>246</v>
       </c>
@@ -26288,7 +26281,7 @@
       <c r="X246" s="2"/>
       <c r="Y246" s="2"/>
     </row>
-    <row r="247" spans="1:25" ht="153.6" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:25" ht="153.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A247" s="4">
         <v>247</v>
       </c>
@@ -26329,7 +26322,7 @@
       <c r="X247" s="2"/>
       <c r="Y247" s="2"/>
     </row>
-    <row r="248" spans="1:25" ht="99.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:25" ht="105" x14ac:dyDescent="0.15">
       <c r="A248" s="4">
         <v>248</v>
       </c>
@@ -26376,7 +26369,7 @@
       <c r="X248" s="2"/>
       <c r="Y248" s="2"/>
     </row>
-    <row r="249" spans="1:25" ht="264.60000000000002" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:25" ht="264.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A249" s="4">
         <v>249</v>
       </c>
@@ -26429,7 +26422,7 @@
       <c r="X249" s="2"/>
       <c r="Y249" s="2"/>
     </row>
-    <row r="250" spans="1:25" ht="285" hidden="1" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:25" ht="300" x14ac:dyDescent="0.15">
       <c r="A250" s="4">
         <v>250</v>
       </c>
@@ -26474,7 +26467,7 @@
       <c r="X250" s="2"/>
       <c r="Y250" s="2"/>
     </row>
-    <row r="251" spans="1:25" ht="142.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:25" ht="165" x14ac:dyDescent="0.15">
       <c r="A251" s="4">
         <v>251</v>
       </c>
@@ -26523,7 +26516,7 @@
       <c r="X251" s="2"/>
       <c r="Y251" s="2"/>
     </row>
-    <row r="252" spans="1:25" ht="127.35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:25" ht="127.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A252" s="4">
         <v>252</v>
       </c>
@@ -26568,7 +26561,7 @@
       <c r="X252" s="2"/>
       <c r="Y252" s="2"/>
     </row>
-    <row r="253" spans="1:25" ht="185.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:25" ht="195" x14ac:dyDescent="0.15">
       <c r="A253" s="4">
         <v>253</v>
       </c>
@@ -26619,7 +26612,7 @@
       <c r="X253" s="2"/>
       <c r="Y253" s="2"/>
     </row>
-    <row r="254" spans="1:25" ht="127.35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:25" ht="127.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A254" s="4">
         <v>254</v>
       </c>
@@ -26662,7 +26655,7 @@
       <c r="X254" s="2"/>
       <c r="Y254" s="2"/>
     </row>
-    <row r="255" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A255" s="4">
         <v>255</v>
       </c>
@@ -26705,7 +26698,7 @@
       <c r="X255" s="2"/>
       <c r="Y255" s="2"/>
     </row>
-    <row r="256" spans="1:25" ht="185.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:25" ht="195" x14ac:dyDescent="0.15">
       <c r="A256" s="4">
         <v>256</v>
       </c>
@@ -26748,7 +26741,7 @@
       <c r="X256" s="2"/>
       <c r="Y256" s="2"/>
     </row>
-    <row r="257" spans="1:25" ht="127.35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:25" ht="127.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A257" s="4">
         <v>257</v>
       </c>
@@ -26791,7 +26784,7 @@
       <c r="X257" s="2"/>
       <c r="Y257" s="2"/>
     </row>
-    <row r="258" spans="1:25" ht="213.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:25" ht="240" x14ac:dyDescent="0.15">
       <c r="A258" s="4">
         <v>258</v>
       </c>
@@ -26834,7 +26827,7 @@
       <c r="X258" s="2"/>
       <c r="Y258" s="2"/>
     </row>
-    <row r="259" spans="1:25" ht="299.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:25" ht="314" x14ac:dyDescent="0.15">
       <c r="A259" s="4">
         <v>259</v>
       </c>
@@ -26881,7 +26874,7 @@
       <c r="X259" s="2"/>
       <c r="Y259" s="2"/>
     </row>
-    <row r="260" spans="1:25" ht="370.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:25" ht="398" x14ac:dyDescent="0.15">
       <c r="A260" s="4">
         <v>260</v>
       </c>
@@ -26924,7 +26917,7 @@
       <c r="X260" s="2"/>
       <c r="Y260" s="2"/>
     </row>
-    <row r="261" spans="1:25" ht="114" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:25" ht="120" x14ac:dyDescent="0.15">
       <c r="A261" s="4">
         <v>261</v>
       </c>
@@ -26971,7 +26964,7 @@
       <c r="X261" s="2"/>
       <c r="Y261" s="2"/>
     </row>
-    <row r="262" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A262" s="4">
         <v>262</v>
       </c>
@@ -27014,7 +27007,7 @@
       <c r="X262" s="2"/>
       <c r="Y262" s="2"/>
     </row>
-    <row r="263" spans="1:25" ht="199.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:25" ht="210" x14ac:dyDescent="0.15">
       <c r="A263" s="4">
         <v>263</v>
       </c>
@@ -27057,7 +27050,7 @@
       <c r="X263" s="2"/>
       <c r="Y263" s="2"/>
     </row>
-    <row r="264" spans="1:25" ht="228" hidden="1" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:25" ht="240" x14ac:dyDescent="0.15">
       <c r="A264" s="4">
         <v>264</v>
       </c>
@@ -27102,7 +27095,7 @@
       <c r="X264" s="2"/>
       <c r="Y264" s="2"/>
     </row>
-    <row r="265" spans="1:25" ht="188.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:25" ht="188.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A265" s="4">
         <v>265</v>
       </c>
@@ -27159,7 +27152,7 @@
       <c r="X265" s="2"/>
       <c r="Y265" s="2"/>
     </row>
-    <row r="266" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A266" s="4">
         <v>266</v>
       </c>
@@ -27212,7 +27205,7 @@
       <c r="X266" s="2"/>
       <c r="Y266" s="2"/>
     </row>
-    <row r="267" spans="1:25" ht="217.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:25" ht="217.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A267" s="4">
         <v>267</v>
       </c>
@@ -27267,7 +27260,7 @@
       <c r="X267" s="2"/>
       <c r="Y267" s="2"/>
     </row>
-    <row r="268" spans="1:25" ht="171" hidden="1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:25" ht="180" x14ac:dyDescent="0.15">
       <c r="A268" s="4">
         <v>268</v>
       </c>
@@ -27324,7 +27317,7 @@
       <c r="X268" s="2"/>
       <c r="Y268" s="2"/>
     </row>
-    <row r="269" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A269" s="4">
         <v>269</v>
       </c>
@@ -27381,7 +27374,7 @@
       <c r="X269" s="2"/>
       <c r="Y269" s="2"/>
     </row>
-    <row r="270" spans="1:25" ht="385.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:25" ht="398" x14ac:dyDescent="0.15">
       <c r="A270" s="4">
         <v>270</v>
       </c>
@@ -27434,7 +27427,7 @@
       <c r="X270" s="2"/>
       <c r="Y270" s="2"/>
     </row>
-    <row r="271" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A271" s="4">
         <v>271</v>
       </c>
@@ -27487,7 +27480,7 @@
       <c r="X271" s="2"/>
       <c r="Y271" s="2"/>
     </row>
-    <row r="272" spans="1:25" ht="342" hidden="1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:25" ht="356" x14ac:dyDescent="0.15">
       <c r="A272" s="4">
         <v>272</v>
       </c>
@@ -27530,7 +27523,7 @@
       <c r="X272" s="2"/>
       <c r="Y272" s="2"/>
     </row>
-    <row r="273" spans="1:25" ht="215.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:25" ht="215" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A273" s="4">
         <v>273</v>
       </c>
@@ -27573,7 +27566,7 @@
       <c r="X273" s="2"/>
       <c r="Y273" s="2"/>
     </row>
-    <row r="274" spans="1:25" ht="231.6" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:25" ht="231.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A274" s="4">
         <v>274</v>
       </c>
@@ -27618,7 +27611,7 @@
       <c r="X274" s="2"/>
       <c r="Y274" s="2"/>
     </row>
-    <row r="275" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A275" s="4">
         <v>275</v>
       </c>
@@ -27661,7 +27654,7 @@
       <c r="X275" s="2"/>
       <c r="Y275" s="2"/>
     </row>
-    <row r="276" spans="1:25" ht="281.85000000000002" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:25" ht="281.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A276" s="4">
         <v>276</v>
       </c>
@@ -27722,7 +27715,7 @@
       <c r="X276" s="2"/>
       <c r="Y276" s="2"/>
     </row>
-    <row r="277" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A277" s="4">
         <v>277</v>
       </c>
@@ -27765,7 +27758,7 @@
       <c r="X277" s="2"/>
       <c r="Y277" s="2"/>
     </row>
-    <row r="278" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A278" s="4">
         <v>278</v>
       </c>
@@ -27808,7 +27801,7 @@
       <c r="X278" s="2"/>
       <c r="Y278" s="2"/>
     </row>
-    <row r="279" spans="1:25" ht="256.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:25" ht="270" x14ac:dyDescent="0.15">
       <c r="A279" s="4">
         <v>279</v>
       </c>
@@ -27855,7 +27848,7 @@
       <c r="X279" s="2"/>
       <c r="Y279" s="2"/>
     </row>
-    <row r="280" spans="1:25" ht="384.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:25" ht="398" x14ac:dyDescent="0.15">
       <c r="A280" s="4">
         <v>280</v>
       </c>
@@ -27916,7 +27909,7 @@
       <c r="X280" s="2"/>
       <c r="Y280" s="2"/>
     </row>
-    <row r="281" spans="1:25" ht="199.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:25" ht="210" x14ac:dyDescent="0.15">
       <c r="A281" s="4">
         <v>281</v>
       </c>
@@ -27963,7 +27956,7 @@
       <c r="X281" s="2"/>
       <c r="Y281" s="2"/>
     </row>
-    <row r="282" spans="1:25" ht="85.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:25" ht="90" x14ac:dyDescent="0.15">
       <c r="A282" s="4">
         <v>282</v>
       </c>
@@ -28008,7 +28001,7 @@
       <c r="X282" s="2"/>
       <c r="Y282" s="2"/>
     </row>
-    <row r="283" spans="1:25" ht="240.6" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:25" ht="240.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A283" s="4">
         <v>283</v>
       </c>
@@ -28051,7 +28044,7 @@
       <c r="X283" s="2"/>
       <c r="Y283" s="2"/>
     </row>
-    <row r="284" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A284" s="4">
         <v>284</v>
       </c>
@@ -28094,7 +28087,7 @@
       <c r="X284" s="2"/>
       <c r="Y284" s="2"/>
     </row>
-    <row r="285" spans="1:25" ht="142.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:25" ht="150" x14ac:dyDescent="0.15">
       <c r="A285" s="4">
         <v>285</v>
       </c>
@@ -28139,7 +28132,7 @@
       <c r="X285" s="2"/>
       <c r="Y285" s="2"/>
     </row>
-    <row r="286" spans="1:25" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:25" ht="120" x14ac:dyDescent="0.15">
       <c r="A286" s="4">
         <v>286</v>
       </c>
@@ -28182,7 +28175,7 @@
       <c r="X286" s="2"/>
       <c r="Y286" s="2"/>
     </row>
-    <row r="287" spans="1:25" ht="171" hidden="1" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:25" ht="180" x14ac:dyDescent="0.15">
       <c r="A287" s="4">
         <v>287</v>
       </c>
@@ -28225,7 +28218,7 @@
       <c r="X287" s="2"/>
       <c r="Y287" s="2"/>
     </row>
-    <row r="288" spans="1:25" ht="213.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:25" ht="225" x14ac:dyDescent="0.15">
       <c r="A288" s="4">
         <v>288</v>
       </c>
@@ -28268,7 +28261,7 @@
       <c r="X288" s="2"/>
       <c r="Y288" s="2"/>
     </row>
-    <row r="289" spans="1:25" ht="270.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:25" ht="285" x14ac:dyDescent="0.15">
       <c r="A289" s="4">
         <v>289</v>
       </c>
@@ -28317,7 +28310,7 @@
       <c r="X289" s="2"/>
       <c r="Y289" s="2"/>
     </row>
-    <row r="290" spans="1:25" ht="185.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:25" ht="195" x14ac:dyDescent="0.15">
       <c r="A290" s="4">
         <v>290</v>
       </c>
@@ -28368,7 +28361,7 @@
       <c r="X290" s="2"/>
       <c r="Y290" s="2"/>
     </row>
-    <row r="291" spans="1:25" ht="384.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:25" ht="398" x14ac:dyDescent="0.15">
       <c r="A291" s="4">
         <v>291</v>
       </c>
@@ -28411,7 +28404,7 @@
       <c r="X291" s="2"/>
       <c r="Y291" s="2"/>
     </row>
-    <row r="292" spans="1:25" ht="128.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:25" ht="135" x14ac:dyDescent="0.15">
       <c r="A292" s="4">
         <v>292</v>
       </c>
@@ -28454,7 +28447,7 @@
       <c r="X292" s="2"/>
       <c r="Y292" s="2"/>
     </row>
-    <row r="293" spans="1:25" ht="312" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:25" ht="312" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A293" s="4">
         <v>293</v>
       </c>
@@ -28511,7 +28504,7 @@
       <c r="X293" s="2"/>
       <c r="Y293" s="2"/>
     </row>
-    <row r="294" spans="1:25" ht="242.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:25" ht="270" x14ac:dyDescent="0.15">
       <c r="A294" s="4">
         <v>294</v>
       </c>
@@ -28554,7 +28547,7 @@
       <c r="X294" s="2"/>
       <c r="Y294" s="2"/>
     </row>
-    <row r="295" spans="1:25" ht="313.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:25" ht="328" x14ac:dyDescent="0.15">
       <c r="A295" s="4">
         <v>295</v>
       </c>
@@ -28597,7 +28590,7 @@
       <c r="X295" s="2"/>
       <c r="Y295" s="2"/>
     </row>
-    <row r="296" spans="1:25" ht="190.35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:25" ht="190.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A296" s="4">
         <v>296</v>
       </c>
@@ -28640,7 +28633,7 @@
       <c r="X296" s="2"/>
       <c r="Y296" s="2"/>
     </row>
-    <row r="297" spans="1:25" ht="409.6" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:25" ht="409.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A297" s="4">
         <v>297</v>
       </c>
@@ -28699,7 +28692,7 @@
       <c r="X297" s="2"/>
       <c r="Y297" s="2"/>
     </row>
-    <row r="298" spans="1:25" ht="166.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:25" ht="166.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A298" s="4">
         <v>298</v>
       </c>
@@ -28752,7 +28745,7 @@
       <c r="X298" s="2"/>
       <c r="Y298" s="2"/>
     </row>
-    <row r="299" spans="1:25" ht="313.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:25" ht="328" x14ac:dyDescent="0.15">
       <c r="A299" s="4">
         <v>299</v>
       </c>
@@ -28795,7 +28788,7 @@
       <c r="X299" s="2"/>
       <c r="Y299" s="2"/>
     </row>
-    <row r="300" spans="1:25" ht="356.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:25" ht="370" x14ac:dyDescent="0.15">
       <c r="A300" s="4">
         <v>300</v>
       </c>
@@ -28838,7 +28831,7 @@
       <c r="X300" s="2"/>
       <c r="Y300" s="2"/>
     </row>
-    <row r="301" spans="1:25" ht="90" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:25" ht="90" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A301" s="4">
         <v>301</v>
       </c>
@@ -28881,7 +28874,7 @@
       <c r="X301" s="2"/>
       <c r="Y301" s="2"/>
     </row>
-    <row r="302" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A302" s="4">
         <v>302</v>
       </c>
@@ -28934,7 +28927,7 @@
       <c r="X302" s="2"/>
       <c r="Y302" s="2"/>
     </row>
-    <row r="303" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A303" s="4">
         <v>303</v>
       </c>
@@ -28991,7 +28984,7 @@
       <c r="X303" s="2"/>
       <c r="Y303" s="2"/>
     </row>
-    <row r="304" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A304" s="4">
         <v>304</v>
       </c>
@@ -29034,7 +29027,7 @@
       <c r="X304" s="2"/>
       <c r="Y304" s="2"/>
     </row>
-    <row r="305" spans="1:25" ht="270.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:25" ht="300" x14ac:dyDescent="0.15">
       <c r="A305" s="4">
         <v>305</v>
       </c>
@@ -29077,7 +29070,7 @@
       <c r="X305" s="2"/>
       <c r="Y305" s="2"/>
     </row>
-    <row r="306" spans="1:25" ht="99" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:25" ht="99" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A306" s="4">
         <v>306</v>
       </c>
@@ -29120,7 +29113,7 @@
       <c r="X306" s="2"/>
       <c r="Y306" s="2"/>
     </row>
-    <row r="307" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A307" s="4">
         <v>307</v>
       </c>
@@ -29179,7 +29172,7 @@
       <c r="X307" s="2"/>
       <c r="Y307" s="2"/>
     </row>
-    <row r="308" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A308" s="4">
         <v>308</v>
       </c>
@@ -29226,7 +29219,7 @@
       <c r="X308" s="2"/>
       <c r="Y308" s="2"/>
     </row>
-    <row r="309" spans="1:25" ht="366.6" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:25" ht="366.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A309" s="4">
         <v>309</v>
       </c>
@@ -29279,7 +29272,7 @@
       <c r="X309" s="2"/>
       <c r="Y309" s="2"/>
     </row>
-    <row r="310" spans="1:25" ht="370.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:25" ht="384" x14ac:dyDescent="0.15">
       <c r="A310" s="4">
         <v>310</v>
       </c>
@@ -29330,7 +29323,7 @@
       <c r="X310" s="2"/>
       <c r="Y310" s="2"/>
     </row>
-    <row r="311" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A311" s="4">
         <v>311</v>
       </c>
@@ -29375,7 +29368,7 @@
       <c r="X311" s="2"/>
       <c r="Y311" s="2"/>
     </row>
-    <row r="312" spans="1:25" ht="167.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:25" ht="167.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A312" s="4">
         <v>312</v>
       </c>
@@ -29420,7 +29413,7 @@
       <c r="X312" s="2"/>
       <c r="Y312" s="2"/>
     </row>
-    <row r="313" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A313" s="4">
         <v>313</v>
       </c>
@@ -29465,7 +29458,7 @@
       <c r="X313" s="2"/>
       <c r="Y313" s="2"/>
     </row>
-    <row r="314" spans="1:25" ht="99" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:25" ht="99" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A314" s="4">
         <v>314</v>
       </c>
@@ -29510,7 +29503,7 @@
       <c r="X314" s="2"/>
       <c r="Y314" s="2"/>
     </row>
-    <row r="315" spans="1:25" ht="99" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:25" ht="99" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A315" s="4">
         <v>315</v>
       </c>
@@ -29551,7 +29544,7 @@
       <c r="X315" s="2"/>
       <c r="Y315" s="2"/>
     </row>
-    <row r="316" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A316" s="4">
         <v>316</v>
       </c>
@@ -29608,7 +29601,7 @@
       <c r="X316" s="2"/>
       <c r="Y316" s="2"/>
     </row>
-    <row r="317" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A317" s="4">
         <v>317</v>
       </c>
@@ -29651,7 +29644,7 @@
       <c r="X317" s="2"/>
       <c r="Y317" s="2"/>
     </row>
-    <row r="318" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A318" s="4">
         <v>318</v>
       </c>
@@ -29706,7 +29699,7 @@
       <c r="X318" s="2"/>
       <c r="Y318" s="2"/>
     </row>
-    <row r="319" spans="1:25" ht="99" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:25" ht="99" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A319" s="4">
         <v>319</v>
       </c>
@@ -29749,7 +29742,7 @@
       <c r="X319" s="2"/>
       <c r="Y319" s="2"/>
     </row>
-    <row r="320" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A320" s="4">
         <v>320</v>
       </c>
@@ -29794,7 +29787,7 @@
       <c r="X320" s="2"/>
       <c r="Y320" s="2"/>
     </row>
-    <row r="321" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A321" s="4">
         <v>321</v>
       </c>
@@ -29837,7 +29830,7 @@
       <c r="X321" s="2"/>
       <c r="Y321" s="2"/>
     </row>
-    <row r="322" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A322" s="4">
         <v>322</v>
       </c>
@@ -29880,7 +29873,7 @@
       <c r="X322" s="2"/>
       <c r="Y322" s="2"/>
     </row>
-    <row r="323" spans="1:25" ht="99" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:25" ht="99" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A323" s="4">
         <v>323</v>
       </c>
@@ -29933,7 +29926,7 @@
       <c r="X323" s="2"/>
       <c r="Y323" s="2"/>
     </row>
-    <row r="324" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A324" s="4">
         <v>324</v>
       </c>
@@ -29976,7 +29969,7 @@
       <c r="X324" s="2"/>
       <c r="Y324" s="2"/>
     </row>
-    <row r="325" spans="1:25" ht="185.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:25" ht="195" x14ac:dyDescent="0.15">
       <c r="A325" s="4">
         <v>325</v>
       </c>
@@ -30027,7 +30020,7 @@
       <c r="X325" s="2"/>
       <c r="Y325" s="2"/>
     </row>
-    <row r="326" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A326" s="4">
         <v>326</v>
       </c>
@@ -30084,7 +30077,7 @@
       <c r="X326" s="2"/>
       <c r="Y326" s="2"/>
     </row>
-    <row r="327" spans="1:25" ht="142.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:25" ht="150" x14ac:dyDescent="0.15">
       <c r="A327" s="4">
         <v>327</v>
       </c>
@@ -30139,7 +30132,7 @@
       <c r="X327" s="2"/>
       <c r="Y327" s="2"/>
     </row>
-    <row r="328" spans="1:25" ht="199.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:25" ht="210" x14ac:dyDescent="0.15">
       <c r="A328" s="4">
         <v>328</v>
       </c>
@@ -30194,7 +30187,7 @@
       <c r="X328" s="2"/>
       <c r="Y328" s="2"/>
     </row>
-    <row r="329" spans="1:25" ht="242.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:25" ht="255" x14ac:dyDescent="0.15">
       <c r="A329" s="4">
         <v>329</v>
       </c>
@@ -30249,7 +30242,7 @@
       <c r="X329" s="2"/>
       <c r="Y329" s="2"/>
     </row>
-    <row r="330" spans="1:25" ht="228" hidden="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:25" ht="240" x14ac:dyDescent="0.15">
       <c r="A330" s="4">
         <v>330</v>
       </c>
@@ -30304,7 +30297,7 @@
       <c r="X330" s="2"/>
       <c r="Y330" s="2"/>
     </row>
-    <row r="331" spans="1:25" ht="184.35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:25" ht="184.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A331" s="4">
         <v>331</v>
       </c>
@@ -30349,7 +30342,7 @@
       <c r="X331" s="2"/>
       <c r="Y331" s="2"/>
     </row>
-    <row r="332" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A332" s="4">
         <v>332</v>
       </c>
@@ -30404,7 +30397,7 @@
       <c r="X332" s="2"/>
       <c r="Y332" s="2"/>
     </row>
-    <row r="333" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A333" s="4">
         <v>333</v>
       </c>
@@ -30451,7 +30444,7 @@
       <c r="X333" s="2"/>
       <c r="Y333" s="2"/>
     </row>
-    <row r="334" spans="1:25" ht="85.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:25" ht="105" x14ac:dyDescent="0.15">
       <c r="A334" s="4">
         <v>334</v>
       </c>
@@ -30496,7 +30489,7 @@
       <c r="X334" s="2"/>
       <c r="Y334" s="2"/>
     </row>
-    <row r="335" spans="1:25" ht="228" hidden="1" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:25" ht="240" x14ac:dyDescent="0.15">
       <c r="A335" s="4">
         <v>335</v>
       </c>
@@ -30539,7 +30532,7 @@
       <c r="X335" s="2"/>
       <c r="Y335" s="2"/>
     </row>
-    <row r="336" spans="1:25" ht="228" hidden="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:25" ht="240" x14ac:dyDescent="0.15">
       <c r="A336" s="4">
         <v>336</v>
       </c>
@@ -30590,7 +30583,7 @@
       <c r="X336" s="2"/>
       <c r="Y336" s="2"/>
     </row>
-    <row r="337" spans="1:25" ht="154.5" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:25" ht="154.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A337" s="4">
         <v>337</v>
       </c>
@@ -30641,7 +30634,7 @@
       <c r="X337" s="2"/>
       <c r="Y337" s="2"/>
     </row>
-    <row r="338" spans="1:25" ht="199.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:25" ht="210" x14ac:dyDescent="0.15">
       <c r="A338" s="4">
         <v>338</v>
       </c>
@@ -30684,7 +30677,7 @@
       <c r="X338" s="2"/>
       <c r="Y338" s="2"/>
     </row>
-    <row r="339" spans="1:25" ht="142.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:25" ht="150" x14ac:dyDescent="0.15">
       <c r="A339" s="4">
         <v>339</v>
       </c>
@@ -30735,7 +30728,7 @@
       <c r="X339" s="2"/>
       <c r="Y339" s="2"/>
     </row>
-    <row r="340" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A340" s="4">
         <v>340</v>
       </c>
@@ -30778,7 +30771,7 @@
       <c r="X340" s="2"/>
       <c r="Y340" s="2"/>
     </row>
-    <row r="341" spans="1:25" ht="199.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:25" ht="210" x14ac:dyDescent="0.15">
       <c r="A341" s="4">
         <v>341</v>
       </c>
@@ -30821,7 +30814,7 @@
       <c r="X341" s="2"/>
       <c r="Y341" s="2"/>
     </row>
-    <row r="342" spans="1:25" ht="213.75" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:25" ht="225" x14ac:dyDescent="0.15">
       <c r="A342" s="4">
         <v>342</v>
       </c>
@@ -30866,7 +30859,7 @@
       <c r="X342" s="2"/>
       <c r="Y342" s="2"/>
     </row>
-    <row r="343" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A343" s="4">
         <v>343</v>
       </c>
@@ -30909,7 +30902,7 @@
       <c r="X343" s="2"/>
       <c r="Y343" s="2"/>
     </row>
-    <row r="344" spans="1:25" ht="285" hidden="1" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:25" ht="300" x14ac:dyDescent="0.15">
       <c r="A344" s="4">
         <v>344</v>
       </c>
@@ -30952,7 +30945,7 @@
       <c r="X344" s="2"/>
       <c r="Y344" s="2"/>
     </row>
-    <row r="345" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A345" s="4">
         <v>345</v>
       </c>
@@ -30995,7 +30988,7 @@
       <c r="X345" s="2"/>
       <c r="Y345" s="2"/>
     </row>
-    <row r="346" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A346" s="4">
         <v>346</v>
       </c>
@@ -31046,7 +31039,7 @@
       <c r="X346" s="2"/>
       <c r="Y346" s="2"/>
     </row>
-    <row r="347" spans="1:25" ht="299.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:25" ht="314" x14ac:dyDescent="0.15">
       <c r="A347" s="4">
         <v>347</v>
       </c>
@@ -31101,7 +31094,7 @@
       <c r="X347" s="2"/>
       <c r="Y347" s="2"/>
     </row>
-    <row r="348" spans="1:25" ht="185.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:25" ht="195" x14ac:dyDescent="0.15">
       <c r="A348" s="4">
         <v>348</v>
       </c>
@@ -31144,7 +31137,7 @@
       <c r="X348" s="2"/>
       <c r="Y348" s="2"/>
     </row>
-    <row r="349" spans="1:25" ht="99.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:25" ht="105" x14ac:dyDescent="0.15">
       <c r="A349" s="4">
         <v>349</v>
       </c>
@@ -31185,7 +31178,7 @@
       <c r="X349" s="2"/>
       <c r="Y349" s="2"/>
     </row>
-    <row r="350" spans="1:25" ht="171" hidden="1" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:25" ht="225" x14ac:dyDescent="0.15">
       <c r="A350" s="4">
         <v>350</v>
       </c>
@@ -31228,7 +31221,7 @@
       <c r="X350" s="2"/>
       <c r="Y350" s="2"/>
     </row>
-    <row r="351" spans="1:25" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A351" s="4">
         <v>351</v>
       </c>
@@ -31277,7 +31270,7 @@
       <c r="X351" s="2"/>
       <c r="Y351" s="2"/>
     </row>
-    <row r="352" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A352" s="4">
         <v>352</v>
       </c>
@@ -31320,7 +31313,7 @@
       <c r="X352" s="2"/>
       <c r="Y352" s="2"/>
     </row>
-    <row r="353" spans="1:25" ht="127.35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:25" ht="127.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A353" s="4">
         <v>353</v>
       </c>
@@ -31373,7 +31366,7 @@
       <c r="X353" s="2"/>
       <c r="Y353" s="2"/>
     </row>
-    <row r="354" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A354" s="4">
         <v>354</v>
       </c>
@@ -31416,7 +31409,7 @@
       <c r="X354" s="2"/>
       <c r="Y354" s="2"/>
     </row>
-    <row r="355" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A355" s="4">
         <v>355</v>
       </c>
@@ -31459,7 +31452,7 @@
       <c r="X355" s="2"/>
       <c r="Y355" s="2"/>
     </row>
-    <row r="356" spans="1:25" ht="185.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:25" ht="210" x14ac:dyDescent="0.15">
       <c r="A356" s="4">
         <v>356</v>
       </c>
@@ -31512,7 +31505,7 @@
       <c r="X356" s="2"/>
       <c r="Y356" s="2"/>
     </row>
-    <row r="357" spans="1:25" ht="156.75" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:25" ht="165" x14ac:dyDescent="0.15">
       <c r="A357" s="4">
         <v>357</v>
       </c>
@@ -31563,7 +31556,7 @@
       <c r="X357" s="2"/>
       <c r="Y357" s="2"/>
     </row>
-    <row r="358" spans="1:25" ht="256.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:25" ht="270" x14ac:dyDescent="0.15">
       <c r="A358" s="4">
         <v>358</v>
       </c>
@@ -31606,7 +31599,7 @@
       <c r="X358" s="2"/>
       <c r="Y358" s="2"/>
     </row>
-    <row r="359" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A359" s="4">
         <v>359</v>
       </c>
@@ -31649,7 +31642,7 @@
       <c r="X359" s="2"/>
       <c r="Y359" s="2"/>
     </row>
-    <row r="360" spans="1:25" ht="356.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:25" ht="370" x14ac:dyDescent="0.15">
       <c r="A360" s="4">
         <v>360</v>
       </c>
@@ -31692,7 +31685,7 @@
       <c r="X360" s="2"/>
       <c r="Y360" s="2"/>
     </row>
-    <row r="361" spans="1:25" ht="185.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:25" ht="195" x14ac:dyDescent="0.15">
       <c r="A361" s="4">
         <v>361</v>
       </c>
@@ -31735,7 +31728,7 @@
       <c r="X361" s="2"/>
       <c r="Y361" s="2"/>
     </row>
-    <row r="362" spans="1:25" ht="213.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:25" ht="225" x14ac:dyDescent="0.15">
       <c r="A362" s="4">
         <v>362</v>
       </c>
@@ -31778,7 +31771,7 @@
       <c r="X362" s="2"/>
       <c r="Y362" s="2"/>
     </row>
-    <row r="363" spans="1:25" ht="199.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:25" ht="210" x14ac:dyDescent="0.15">
       <c r="A363" s="4">
         <v>363</v>
       </c>
@@ -31821,7 +31814,7 @@
       <c r="X363" s="2"/>
       <c r="Y363" s="2"/>
     </row>
-    <row r="364" spans="1:25" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A364" s="4">
         <v>364</v>
       </c>
@@ -31874,7 +31867,7 @@
       <c r="X364" s="2"/>
       <c r="Y364" s="2"/>
     </row>
-    <row r="365" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A365" s="4">
         <v>365</v>
       </c>
@@ -31927,7 +31920,7 @@
       <c r="X365" s="2"/>
       <c r="Y365" s="2"/>
     </row>
-    <row r="366" spans="1:25" ht="171" hidden="1" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:25" ht="180" x14ac:dyDescent="0.15">
       <c r="A366" s="4">
         <v>366</v>
       </c>
@@ -31970,7 +31963,7 @@
       <c r="X366" s="2"/>
       <c r="Y366" s="2"/>
     </row>
-    <row r="367" spans="1:25" ht="85.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:25" ht="90" x14ac:dyDescent="0.15">
       <c r="A367" s="4">
         <v>367</v>
       </c>
@@ -32015,7 +32008,7 @@
       <c r="X367" s="2"/>
       <c r="Y367" s="2"/>
     </row>
-    <row r="368" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A368" s="4">
         <v>368</v>
       </c>
@@ -32058,7 +32051,7 @@
       <c r="X368" s="2"/>
       <c r="Y368" s="2"/>
     </row>
-    <row r="369" spans="1:25" ht="242.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:25" ht="255" x14ac:dyDescent="0.15">
       <c r="A369" s="4">
         <v>369</v>
       </c>
@@ -32101,7 +32094,7 @@
       <c r="X369" s="2"/>
       <c r="Y369" s="2"/>
     </row>
-    <row r="370" spans="1:25" ht="114" hidden="1" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:25" ht="120" x14ac:dyDescent="0.15">
       <c r="A370" s="4">
         <v>370</v>
       </c>
@@ -32144,7 +32137,7 @@
       <c r="X370" s="2"/>
       <c r="Y370" s="2"/>
     </row>
-    <row r="371" spans="1:25" ht="185.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:25" ht="210" x14ac:dyDescent="0.15">
       <c r="A371" s="4">
         <v>371</v>
       </c>
@@ -32187,7 +32180,7 @@
       <c r="X371" s="2"/>
       <c r="Y371" s="2"/>
     </row>
-    <row r="372" spans="1:25" ht="185.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:25" ht="195" x14ac:dyDescent="0.15">
       <c r="A372" s="4">
         <v>372</v>
       </c>
@@ -32230,7 +32223,7 @@
       <c r="X372" s="2"/>
       <c r="Y372" s="2"/>
     </row>
-    <row r="373" spans="1:25" ht="370.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:25" ht="384" x14ac:dyDescent="0.15">
       <c r="A373" s="4">
         <v>373</v>
       </c>
@@ -32273,7 +32266,7 @@
       <c r="X373" s="2"/>
       <c r="Y373" s="2"/>
     </row>
-    <row r="374" spans="1:25" ht="232.35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:25" ht="232.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A374" s="4">
         <v>374</v>
       </c>
@@ -32322,7 +32315,7 @@
       <c r="X374" s="2"/>
       <c r="Y374" s="2"/>
     </row>
-    <row r="375" spans="1:25" ht="213.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:25" ht="225" x14ac:dyDescent="0.15">
       <c r="A375" s="4">
         <v>375</v>
       </c>
@@ -32377,7 +32370,7 @@
       <c r="X375" s="2"/>
       <c r="Y375" s="2"/>
     </row>
-    <row r="376" spans="1:25" ht="128.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:25" ht="135" x14ac:dyDescent="0.15">
       <c r="A376" s="4">
         <v>376</v>
       </c>
@@ -32428,7 +32421,7 @@
       <c r="X376" s="2"/>
       <c r="Y376" s="2"/>
     </row>
-    <row r="377" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A377" s="4">
         <v>377</v>
       </c>
@@ -32481,7 +32474,7 @@
       <c r="X377" s="2"/>
       <c r="Y377" s="2"/>
     </row>
-    <row r="378" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A378" s="4">
         <v>378</v>
       </c>
@@ -32524,7 +32517,7 @@
       <c r="X378" s="2"/>
       <c r="Y378" s="2"/>
     </row>
-    <row r="379" spans="1:25" ht="85.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:25" ht="90" x14ac:dyDescent="0.15">
       <c r="A379" s="4">
         <v>379</v>
       </c>
@@ -32567,7 +32560,7 @@
       <c r="X379" s="2"/>
       <c r="Y379" s="2"/>
     </row>
-    <row r="380" spans="1:25" ht="174" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:25" ht="174" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A380" s="4">
         <v>380</v>
       </c>
@@ -32610,7 +32603,7 @@
       <c r="X380" s="2"/>
       <c r="Y380" s="2"/>
     </row>
-    <row r="381" spans="1:25" ht="113.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:25" ht="113" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A381" s="4">
         <v>381</v>
       </c>
@@ -32663,7 +32656,7 @@
       <c r="X381" s="2"/>
       <c r="Y381" s="2"/>
     </row>
-    <row r="382" spans="1:25" ht="299.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:25" ht="314" x14ac:dyDescent="0.15">
       <c r="A382" s="4">
         <v>382</v>
       </c>
@@ -32720,7 +32713,7 @@
       <c r="X382" s="2"/>
       <c r="Y382" s="2"/>
     </row>
-    <row r="383" spans="1:25" ht="370.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:25" ht="384" x14ac:dyDescent="0.15">
       <c r="A383" s="4">
         <v>383</v>
       </c>
@@ -32763,7 +32756,7 @@
       <c r="X383" s="2"/>
       <c r="Y383" s="2"/>
     </row>
-    <row r="384" spans="1:25" ht="142.5" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:25" ht="165" x14ac:dyDescent="0.15">
       <c r="A384" s="4">
         <v>384</v>
       </c>
@@ -32814,7 +32807,7 @@
       <c r="X384" s="2"/>
       <c r="Y384" s="2"/>
     </row>
-    <row r="385" spans="1:25" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:25" ht="118.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A385" s="4">
         <v>385</v>
       </c>
@@ -32859,7 +32852,7 @@
       <c r="X385" s="2"/>
       <c r="Y385" s="2"/>
     </row>
-    <row r="386" spans="1:25" ht="327.75" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:25" ht="356" x14ac:dyDescent="0.15">
       <c r="A386" s="4">
         <v>386</v>
       </c>
@@ -32908,7 +32901,7 @@
       <c r="X386" s="2"/>
       <c r="Y386" s="2"/>
     </row>
-    <row r="387" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A387" s="4">
         <v>387</v>
       </c>
@@ -32949,7 +32942,7 @@
       <c r="X387" s="2"/>
       <c r="Y387" s="2"/>
     </row>
-    <row r="388" spans="1:25" ht="370.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:25" ht="384" x14ac:dyDescent="0.15">
       <c r="A388" s="4">
         <v>388</v>
       </c>
@@ -33000,7 +32993,7 @@
       <c r="X388" s="2"/>
       <c r="Y388" s="2"/>
     </row>
-    <row r="389" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A389" s="4">
         <v>389</v>
       </c>
@@ -33053,7 +33046,7 @@
       <c r="X389" s="2"/>
       <c r="Y389" s="2"/>
     </row>
-    <row r="390" spans="1:25" ht="185.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:25" ht="195" x14ac:dyDescent="0.15">
       <c r="A390" s="4">
         <v>390</v>
       </c>
@@ -33108,7 +33101,7 @@
       <c r="X390" s="2"/>
       <c r="Y390" s="2"/>
     </row>
-    <row r="391" spans="1:25" ht="213.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:25" ht="240" x14ac:dyDescent="0.15">
       <c r="A391" s="4">
         <v>391</v>
       </c>
@@ -33151,7 +33144,7 @@
       <c r="X391" s="2"/>
       <c r="Y391" s="2"/>
     </row>
-    <row r="392" spans="1:25" ht="199.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:25" ht="210" x14ac:dyDescent="0.15">
       <c r="A392" s="4">
         <v>392</v>
       </c>
@@ -33194,7 +33187,7 @@
       <c r="X392" s="2"/>
       <c r="Y392" s="2"/>
     </row>
-    <row r="393" spans="1:25" ht="99.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:25" ht="105" x14ac:dyDescent="0.15">
       <c r="A393" s="4">
         <v>393</v>
       </c>
@@ -33237,7 +33230,7 @@
       <c r="X393" s="2"/>
       <c r="Y393" s="2"/>
     </row>
-    <row r="394" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A394" s="4">
         <v>394</v>
       </c>
@@ -33290,7 +33283,7 @@
       <c r="X394" s="2"/>
       <c r="Y394" s="2"/>
     </row>
-    <row r="395" spans="1:25" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A395" s="4">
         <v>395</v>
       </c>
@@ -33345,7 +33338,7 @@
       <c r="X395" s="2"/>
       <c r="Y395" s="2"/>
     </row>
-    <row r="396" spans="1:25" ht="256.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:25" ht="270" x14ac:dyDescent="0.15">
       <c r="A396" s="4">
         <v>396</v>
       </c>
@@ -33388,7 +33381,7 @@
       <c r="X396" s="2"/>
       <c r="Y396" s="2"/>
     </row>
-    <row r="397" spans="1:25" ht="71.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:25" ht="75" x14ac:dyDescent="0.15">
       <c r="A397" s="4">
         <v>397</v>
       </c>
@@ -33431,7 +33424,7 @@
       <c r="X397" s="2"/>
       <c r="Y397" s="2"/>
     </row>
-    <row r="398" spans="1:25" ht="99.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:25" ht="105" x14ac:dyDescent="0.15">
       <c r="A398" s="4">
         <v>398</v>
       </c>
@@ -33474,7 +33467,7 @@
       <c r="X398" s="2"/>
       <c r="Y398" s="2"/>
     </row>
-    <row r="399" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A399" s="4">
         <v>399</v>
       </c>
@@ -33517,7 +33510,7 @@
       <c r="X399" s="2"/>
       <c r="Y399" s="2"/>
     </row>
-    <row r="400" spans="1:25" ht="185.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:25" ht="195" x14ac:dyDescent="0.15">
       <c r="A400" s="4">
         <v>400</v>
       </c>
@@ -33560,7 +33553,7 @@
       <c r="X400" s="2"/>
       <c r="Y400" s="2"/>
     </row>
-    <row r="401" spans="1:25" ht="242.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:25" ht="255" x14ac:dyDescent="0.15">
       <c r="A401" s="4">
         <v>401</v>
       </c>
@@ -33603,7 +33596,7 @@
       <c r="X401" s="2"/>
       <c r="Y401" s="2"/>
     </row>
-    <row r="402" spans="1:25" ht="161.1" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:25" ht="161" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A402" s="4">
         <v>402</v>
       </c>
@@ -33646,7 +33639,7 @@
       <c r="X402" s="2"/>
       <c r="Y402" s="2"/>
     </row>
-    <row r="403" spans="1:25" ht="242.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:25" ht="255" x14ac:dyDescent="0.15">
       <c r="A403" s="4">
         <v>403</v>
       </c>
@@ -33703,7 +33696,7 @@
       <c r="X403" s="2"/>
       <c r="Y403" s="2"/>
     </row>
-    <row r="404" spans="1:25" ht="128.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:25" ht="135" x14ac:dyDescent="0.15">
       <c r="A404" s="4">
         <v>404</v>
       </c>
@@ -33758,7 +33751,7 @@
       <c r="X404" s="2"/>
       <c r="Y404" s="2"/>
     </row>
-    <row r="405" spans="1:25" ht="327.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:25" ht="342" x14ac:dyDescent="0.15">
       <c r="A405" s="4">
         <v>405</v>
       </c>
@@ -33801,7 +33794,7 @@
       <c r="X405" s="2"/>
       <c r="Y405" s="2"/>
     </row>
-    <row r="406" spans="1:25" ht="142.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:25" ht="150" x14ac:dyDescent="0.15">
       <c r="A406" s="4">
         <v>406</v>
       </c>
@@ -33852,7 +33845,7 @@
       <c r="X406" s="2"/>
       <c r="Y406" s="2"/>
     </row>
-    <row r="407" spans="1:25" ht="185.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:25" ht="195" x14ac:dyDescent="0.15">
       <c r="A407" s="4">
         <v>407</v>
       </c>
@@ -33901,7 +33894,7 @@
       <c r="X407" s="2"/>
       <c r="Y407" s="2"/>
     </row>
-    <row r="408" spans="1:25" ht="384.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:25" ht="398" x14ac:dyDescent="0.15">
       <c r="A408" s="4">
         <v>408</v>
       </c>
@@ -33944,7 +33937,7 @@
       <c r="X408" s="2"/>
       <c r="Y408" s="2"/>
     </row>
-    <row r="409" spans="1:25" ht="85.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:25" ht="90" x14ac:dyDescent="0.15">
       <c r="A409" s="4">
         <v>409</v>
       </c>
@@ -33995,7 +33988,7 @@
       <c r="X409" s="2"/>
       <c r="Y409" s="2"/>
     </row>
-    <row r="410" spans="1:25" ht="384.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A410" s="4">
         <v>410</v>
       </c>
@@ -34038,7 +34031,7 @@
       <c r="X410" s="2"/>
       <c r="Y410" s="2"/>
     </row>
-    <row r="411" spans="1:25" ht="109.35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:25" ht="109.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A411" s="4">
         <v>411</v>
       </c>
@@ -34083,7 +34076,7 @@
       <c r="X411" s="2"/>
       <c r="Y411" s="2"/>
     </row>
-    <row r="412" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A412" s="4">
         <v>412</v>
       </c>
@@ -34126,7 +34119,7 @@
       <c r="X412" s="2"/>
       <c r="Y412" s="2"/>
     </row>
-    <row r="413" spans="1:25" ht="409.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:25" ht="409.6" x14ac:dyDescent="0.15">
       <c r="A413" s="4">
         <v>413</v>
       </c>
@@ -34169,7 +34162,7 @@
       <c r="X413" s="2"/>
       <c r="Y413" s="2"/>
     </row>
-    <row r="414" spans="1:25" ht="327.75" hidden="1" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:25" ht="342" x14ac:dyDescent="0.15">
       <c r="A414" s="4">
         <v>414</v>
       </c>
@@ -34210,7 +34203,7 @@
       <c r="X414" s="2"/>
       <c r="Y414" s="2"/>
     </row>
-    <row r="415" spans="1:25" ht="185.25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:25" ht="195" x14ac:dyDescent="0.15">
       <c r="A415" s="4">
         <v>415</v>
       </c>
@@ -34259,7 +34252,7 @@
       <c r="X415" s="2"/>
       <c r="Y415" s="2"/>
     </row>
-    <row r="416" spans="1:25" ht="110.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:25" ht="110.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A416" s="4">
         <v>416</v>
       </c>
@@ -34296,7 +34289,7 @@
       <c r="X416" s="2"/>
       <c r="Y416" s="2"/>
     </row>
-    <row r="417" spans="1:25" ht="409.35" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:25" ht="409.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A417" s="4">
         <v>417</v>
       </c>
@@ -34337,7 +34330,7 @@
       <c r="X417" s="2"/>
       <c r="Y417" s="2"/>
     </row>
-    <row r="418" spans="1:25" ht="228" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:25" ht="240" x14ac:dyDescent="0.15">
       <c r="A418" s="4">
         <v>418</v>
       </c>
@@ -34390,7 +34383,7 @@
       <c r="X418" s="2"/>
       <c r="Y418" s="2"/>
     </row>
-    <row r="419" spans="1:25" ht="200.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:25" ht="200.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A419" s="4">
         <v>419</v>
       </c>
@@ -34445,7 +34438,7 @@
       <c r="X419" s="2"/>
       <c r="Y419" s="2"/>
     </row>
-    <row r="420" spans="1:25" ht="102.6" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:25" ht="102.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A420" s="4">
         <v>420</v>
       </c>
@@ -34484,7 +34477,7 @@
       <c r="X420" s="2"/>
       <c r="Y420" s="2"/>
     </row>
-    <row r="421" spans="1:25" ht="199.5" hidden="1" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:25" ht="210" x14ac:dyDescent="0.15">
       <c r="A421" s="4">
         <v>421</v>
       </c>
@@ -34519,7 +34512,7 @@
       <c r="X421" s="2"/>
       <c r="Y421" s="2"/>
     </row>
-    <row r="422" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A422" s="4"/>
       <c r="B422" s="12"/>
       <c r="C422" s="12"/>
@@ -34544,7 +34537,7 @@
       <c r="V422" s="14"/>
       <c r="W422" s="12"/>
     </row>
-    <row r="423" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A423" s="12"/>
       <c r="B423" s="12"/>
       <c r="C423" s="12"/>
@@ -34569,7 +34562,7 @@
       <c r="V423" s="14"/>
       <c r="W423" s="12"/>
     </row>
-    <row r="424" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A424" s="12"/>
       <c r="B424" s="12"/>
       <c r="C424" s="12"/>
@@ -34594,7 +34587,7 @@
       <c r="V424" s="14"/>
       <c r="W424" s="12"/>
     </row>
-    <row r="425" spans="1:25" hidden="1" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A425" s="12"/>
       <c r="B425" s="12"/>
       <c r="C425" s="12"/>
@@ -34637,13 +34630,13 @@
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="33.5" customWidth="1"/>
-    <col min="2" max="2" width="69.625" customWidth="1"/>
+    <col min="2" max="2" width="69.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" s="49" t="s">
         <v>1036</v>
       </c>
@@ -34651,7 +34644,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>993</v>
       </c>
@@ -34659,7 +34652,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>1024</v>
       </c>
@@ -34667,7 +34660,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>632</v>
       </c>
@@ -34675,7 +34668,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>1019</v>
       </c>
@@ -34683,7 +34676,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>1029</v>
       </c>
@@ -34691,7 +34684,7 @@
         <v>1030</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="57" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" ht="60" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>1031</v>
       </c>
@@ -34699,7 +34692,7 @@
         <v>1032</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>86</v>
       </c>
@@ -34707,7 +34700,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>1034</v>
       </c>
@@ -34715,7 +34708,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.15">
       <c r="A14" s="50" t="s">
         <v>1039</v>
       </c>
@@ -34723,7 +34716,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>1</v>
       </c>
@@ -34731,7 +34724,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>2</v>
       </c>
@@ -34739,7 +34732,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>3</v>
       </c>
@@ -34747,7 +34740,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>4</v>
       </c>
@@ -34755,7 +34748,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>1045</v>
       </c>
@@ -34763,7 +34756,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.15">
       <c r="A23" s="50" t="s">
         <v>104</v>
       </c>
@@ -34771,22 +34764,22 @@
         <v>1186</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" s="66" t="s">
         <v>830</v>
       </c>
@@ -34794,7 +34787,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" s="66" t="s">
         <v>1176</v>
       </c>
@@ -34802,7 +34795,7 @@
         <v>1185</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" s="66" t="s">
         <v>1187</v>
       </c>
@@ -34823,7 +34816,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>

</xml_diff>